<commit_message>
added in-excel defined sources
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\panos\repos\DocumentCreator\DocumentCreator.Tests\Resources\"/>
@@ -457,6 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1511,10 +1512,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,6 +2601,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="C2:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
added support for DAY, MONTH,YEAR, DAYS, DATEDIF functions
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\panos\repos\DocumentCreator\DocumentCreator.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\panos\repos\DocumentCreator\DocumentCreator.Tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMPARISON" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="32">
   <si>
     <t>"A"</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>DATEDIF</t>
+  </si>
+  <si>
+    <t>DAYS</t>
   </si>
 </sst>
 </file>
@@ -1536,10 +1551,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,7 +2679,7 @@
         <v>43939</v>
       </c>
       <c r="C91" s="6" t="str">
-        <f t="shared" ref="C91:C104" ca="1" si="10">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B91),"""","\"""),";",","),""", """,IFERROR(B91,IF(ISNA(B91),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C91:C108" ca="1" si="10">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B91),"""","\"""),";",","),""", """,IFERROR(B91,IF(ISNA(B91),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=DATE(2020,4,18)", "43939");</v>
       </c>
     </row>
@@ -2827,6 +2842,564 @@
       <c r="C104" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
         <v>AssertExpression("=TIME(11,6,43)+4,32", "4,78299768518519");</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="8"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>27</v>
+      </c>
+      <c r="B106">
+        <f>DAY(1)</f>
+        <v>1</v>
+      </c>
+      <c r="C106" s="6" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>AssertExpression("=DAY(1)", "1");</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>27</v>
+      </c>
+      <c r="B107">
+        <f>DAY(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C107" s="6" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>AssertExpression("=DAY(0)", "0");</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>27</v>
+      </c>
+      <c r="B108" t="e">
+        <f>DAY(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C108" s="6" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v>AssertExpression("=DAY(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>27</v>
+      </c>
+      <c r="B109">
+        <f>DAY(39448)</f>
+        <v>1</v>
+      </c>
+      <c r="C109" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B109),"""","\"""),";",","),""", """,IFERROR(B109,IF(ISNA(B109),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAY(39448)", "1");</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>27</v>
+      </c>
+      <c r="B110">
+        <f>DAY(39448.999)</f>
+        <v>1</v>
+      </c>
+      <c r="C110" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B110),"""","\"""),";",","),""", """,IFERROR(B110,IF(ISNA(B110),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAY(39448,999)", "1");</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>27</v>
+      </c>
+      <c r="B111">
+        <f>DAY("18/4/2020")</f>
+        <v>18</v>
+      </c>
+      <c r="C111" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B111),"""","\"""),";",","),""", """,IFERROR(B111,IF(ISNA(B111),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAY(\"18/4/2020\")", "18");</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>27</v>
+      </c>
+      <c r="B112">
+        <f>DAY("18/4/2020 10:10:20")</f>
+        <v>18</v>
+      </c>
+      <c r="C112" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B112),"""","\"""),";",","),""", """,IFERROR(B112,IF(ISNA(B112),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAY(\"18/4/2020 10:10:20\")", "18");</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="8"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114">
+        <f>MONTH(1)</f>
+        <v>1</v>
+      </c>
+      <c r="C114" s="6" t="str">
+        <f t="shared" ref="C114:C120" ca="1" si="11">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B114),"""","\"""),";",","),""", """,IFERROR(B114,IF(ISNA(B114),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MONTH(1)", "1");</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115">
+        <f>MONTH(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C115" s="6" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>AssertExpression("=MONTH(0)", "1");</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" t="e">
+        <f>MONTH(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C116" s="6" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>AssertExpression("=MONTH(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117">
+        <f>MONTH(39448)</f>
+        <v>1</v>
+      </c>
+      <c r="C117" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B117),"""","\"""),";",","),""", """,IFERROR(B117,IF(ISNA(B117),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MONTH(39448)", "1");</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>28</v>
+      </c>
+      <c r="B118">
+        <f>MONTH(39448.999)</f>
+        <v>1</v>
+      </c>
+      <c r="C118" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B118),"""","\"""),";",","),""", """,IFERROR(B118,IF(ISNA(B118),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MONTH(39448,999)", "1");</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B119">
+        <f>MONTH("18/4/2020")</f>
+        <v>4</v>
+      </c>
+      <c r="C119" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B119),"""","\"""),";",","),""", """,IFERROR(B119,IF(ISNA(B119),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MONTH(\"18/4/2020\")", "4");</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>28</v>
+      </c>
+      <c r="B120">
+        <f>MONTH("18/4/2020 10:10:20")</f>
+        <v>4</v>
+      </c>
+      <c r="C120" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B120),"""","\"""),";",","),""", """,IFERROR(B120,IF(ISNA(B120),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MONTH(\"18/4/2020 10:10:20\")", "4");</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="8"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>29</v>
+      </c>
+      <c r="B122">
+        <f>YEAR(1)</f>
+        <v>1900</v>
+      </c>
+      <c r="C122" s="6" t="str">
+        <f t="shared" ref="C122:C128" ca="1" si="12">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B122),"""","\"""),";",","),""", """,IFERROR(B122,IF(ISNA(B122),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=YEAR(1)", "1900");</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>29</v>
+      </c>
+      <c r="B123">
+        <f>YEAR(0)</f>
+        <v>1900</v>
+      </c>
+      <c r="C123" s="6" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v>AssertExpression("=YEAR(0)", "1900");</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>29</v>
+      </c>
+      <c r="B124" t="e">
+        <f>YEAR(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C124" s="6" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v>AssertExpression("=YEAR(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>29</v>
+      </c>
+      <c r="B125">
+        <f>YEAR(39448)</f>
+        <v>2008</v>
+      </c>
+      <c r="C125" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B125),"""","\"""),";",","),""", """,IFERROR(B125,IF(ISNA(B125),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=YEAR(39448)", "2008");</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>29</v>
+      </c>
+      <c r="B126">
+        <f>YEAR(40178.99999)</f>
+        <v>2009</v>
+      </c>
+      <c r="C126" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B126),"""","\"""),";",","),""", """,IFERROR(B126,IF(ISNA(B126),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=YEAR(40178,99999)", "2009");</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>29</v>
+      </c>
+      <c r="B127">
+        <f>YEAR("18/4/2020")</f>
+        <v>2020</v>
+      </c>
+      <c r="C127" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B127),"""","\"""),";",","),""", """,IFERROR(B127,IF(ISNA(B127),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=YEAR(\"18/4/2020\")", "2020");</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>29</v>
+      </c>
+      <c r="B128">
+        <f>YEAR("18/4/2020 10:10:20")</f>
+        <v>2020</v>
+      </c>
+      <c r="C128" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B128),"""","\"""),";",","),""", """,IFERROR(B128,IF(ISNA(B128),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=YEAR(\"18/4/2020 10:10:20\")", "2020");</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="8"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>31</v>
+      </c>
+      <c r="B130">
+        <f>_xlfn.DAYS(0,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C130" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B130),"""","\"""),";",","),""", """,IFERROR(B130,IF(ISNA(B130),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(0,0)", "0");</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>31</v>
+      </c>
+      <c r="B131">
+        <f>_xlfn.DAYS(1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C131" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B131),"""","\"""),";",","),""", """,IFERROR(B131,IF(ISNA(B131),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(1,0)", "1");</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>31</v>
+      </c>
+      <c r="B132">
+        <f>_xlfn.DAYS(2,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C132" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B132),"""","\"""),";",","),""", """,IFERROR(B132,IF(ISNA(B132),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(2,1)", "1");</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+      <c r="B133">
+        <f>_xlfn.DAYS(1,2)</f>
+        <v>-1</v>
+      </c>
+      <c r="C133" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B133),"""","\"""),";",","),""", """,IFERROR(B133,IF(ISNA(B133),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(1,2)", "-1");</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>31</v>
+      </c>
+      <c r="B134">
+        <f>_xlfn.DAYS(40002.999,40000.222)</f>
+        <v>2</v>
+      </c>
+      <c r="C134" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B134),"""","\"""),";",","),""", """,IFERROR(B134,IF(ISNA(B134),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(40002,999,40000,222)", "2");</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>31</v>
+      </c>
+      <c r="B135">
+        <f>_xlfn.DAYS("20/4/2020","18/4/2020")</f>
+        <v>2</v>
+      </c>
+      <c r="C135" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B135),"""","\"""),";",","),""", """,IFERROR(B135,IF(ISNA(B135),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(\"20/4/2020\",\"18/4/2020\")", "2");</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>31</v>
+      </c>
+      <c r="B136">
+        <f>_xlfn.DAYS("23/5/2020",43967)</f>
+        <v>7</v>
+      </c>
+      <c r="C136" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B136),"""","\"""),";",","),""", """,IFERROR(B136,IF(ISNA(B136),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(\"23/5/2020\",43967)", "7");</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>31</v>
+      </c>
+      <c r="B137">
+        <f>_xlfn.DAYS(43967,"23/5/2020")</f>
+        <v>-7</v>
+      </c>
+      <c r="C137" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B137),"""","\"""),";",","),""", """,IFERROR(B137,IF(ISNA(B137),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(43967,\"23/5/2020\")", "-7");</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>31</v>
+      </c>
+      <c r="B138">
+        <f>_xlfn.DAYS(43967.99999,43967)</f>
+        <v>0</v>
+      </c>
+      <c r="C138" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B138),"""","\"""),";",","),""", """,IFERROR(B138,IF(ISNA(B138),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(43967,99999,43967)", "0");</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>31</v>
+      </c>
+      <c r="B139">
+        <f>_xlfn.DAYS(43967,43967.99999)</f>
+        <v>0</v>
+      </c>
+      <c r="C139" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B139),"""","\"""),";",","),""", """,IFERROR(B139,IF(ISNA(B139),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(43967,43967,99999)", "0");</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>31</v>
+      </c>
+      <c r="B140" t="e">
+        <f>_xlfn.DAYS(43967,-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C140" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B140),"""","\"""),";",","),""", """,IFERROR(B140,IF(ISNA(B140),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(43967,-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>31</v>
+      </c>
+      <c r="B141" t="e">
+        <f>_xlfn.DAYS("32/4/2020","18/4/2020")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C141" s="6" t="str">
+        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B141),"""","\"""),";",","),""", """,IFERROR(B141,IF(ISNA(B141),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DAYS(\"32/4/2020\",\"18/4/2020\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="8"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>30</v>
+      </c>
+      <c r="B143">
+        <f>DATEDIF("1/6/2001", "15/8/2002", "Y")</f>
+        <v>1</v>
+      </c>
+      <c r="C143" s="6" t="str">
+        <f t="shared" ref="C143:C150" ca="1" si="13">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B143),"""","\"""),";",","),""", """,IFERROR(B143,IF(ISNA(B143),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"Y\")", "1");</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>30</v>
+      </c>
+      <c r="B144">
+        <f>DATEDIF("1/6/2001", "15/8/2002", "M")</f>
+        <v>14</v>
+      </c>
+      <c r="C144" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"M\")", "14");</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>30</v>
+      </c>
+      <c r="B145">
+        <f>DATEDIF("1/6/2001", "15/8/2002", "D")</f>
+        <v>440</v>
+      </c>
+      <c r="C145" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"D\")", "440");</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>30</v>
+      </c>
+      <c r="B146">
+        <f>DATEDIF("1/6/2001", "15/8/2002", "MD")</f>
+        <v>14</v>
+      </c>
+      <c r="C146" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"MD\")", "14");</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>30</v>
+      </c>
+      <c r="B147">
+        <f>DATEDIF("1/6/2001", "15/8/2002", "YM")</f>
+        <v>2</v>
+      </c>
+      <c r="C147" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"YM\")", "2");</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>30</v>
+      </c>
+      <c r="B148">
+        <f>DATEDIF("1/6/2001", "15/8/2002", "YD")</f>
+        <v>75</v>
+      </c>
+      <c r="C148" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"YD\")", "75");</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>30</v>
+      </c>
+      <c r="B149" t="e">
+        <f>DATEDIF("1/6/2003", "15/8/2002", "YD")</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C149" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2003\", \"15/8/2002\", \"YD\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>30</v>
+      </c>
+      <c r="B150">
+        <f>DATEDIF("1/1/2001", "1/1/2003", "Y")</f>
+        <v>2</v>
+      </c>
+      <c r="C150" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/1/2001\", \"1/1/2003\", \"Y\")", "2");</v>
       </c>
     </row>
   </sheetData>
@@ -2840,7 +3413,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added support for ENCODEURL, WEBSERVICE,  FILTERXML and TIMEVALUE functions
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="37">
   <si>
     <t>"A"</t>
   </si>
@@ -122,6 +122,21 @@
   </si>
   <si>
     <t>DAYS</t>
+  </si>
+  <si>
+    <t>HOUR</t>
+  </si>
+  <si>
+    <t>MINUTE</t>
+  </si>
+  <si>
+    <t>SECOND</t>
+  </si>
+  <si>
+    <t>DATEVALUE</t>
+  </si>
+  <si>
+    <t>TIMEVALUE</t>
   </si>
 </sst>
 </file>
@@ -1551,10 +1566,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="6" t="str">
-        <f t="shared" ref="C143:C150" ca="1" si="13">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B143),"""","\"""),";",","),""", """,IFERROR(B143,IF(ISNA(B143),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C143:C174" ca="1" si="13">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B143),"""","\"""),";",","),""", """,IFERROR(B143,IF(ISNA(B143),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"Y\")", "1");</v>
       </c>
     </row>
@@ -3400,6 +3415,798 @@
       <c r="C150" s="6" t="str">
         <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DATEDIF(\"1/1/2001\", \"1/1/2003\", \"Y\")", "2");</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>30</v>
+      </c>
+      <c r="B151">
+        <f>DATEDIF("1/6/2019", "31/5/2020", "Y")</f>
+        <v>0</v>
+      </c>
+      <c r="C151" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"Y\")", "0");</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>30</v>
+      </c>
+      <c r="B152">
+        <f>DATEDIF("1/6/2019", "1/6/2020", "Y")</f>
+        <v>1</v>
+      </c>
+      <c r="C152" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"Y\")", "1");</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>30</v>
+      </c>
+      <c r="B153">
+        <f>DATEDIF("1/6/2020", "31/5/2021", "Y")</f>
+        <v>0</v>
+      </c>
+      <c r="C153" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"Y\")", "0");</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>30</v>
+      </c>
+      <c r="B154">
+        <f>DATEDIF("1/6/2020", "1/6/2021", "Y")</f>
+        <v>1</v>
+      </c>
+      <c r="C154" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"Y\")", "1");</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>30</v>
+      </c>
+      <c r="B155">
+        <f>DATEDIF("1/6/2019", "31/5/2020", "M")</f>
+        <v>11</v>
+      </c>
+      <c r="C155" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"M\")", "11");</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>30</v>
+      </c>
+      <c r="B156">
+        <f>DATEDIF("1/6/2019", "1/6/2020", "m")</f>
+        <v>12</v>
+      </c>
+      <c r="C156" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"m\")", "12");</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>30</v>
+      </c>
+      <c r="B157">
+        <f>DATEDIF("1/6/2020", "31/5/2021", "m")</f>
+        <v>11</v>
+      </c>
+      <c r="C157" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"m\")", "11");</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>30</v>
+      </c>
+      <c r="B158">
+        <f>DATEDIF("1/6/2020", "1/6/2021", "m")</f>
+        <v>12</v>
+      </c>
+      <c r="C158" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"m\")", "12");</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>30</v>
+      </c>
+      <c r="B159">
+        <f>DATEDIF("1/6/2019", "31/5/2020", "D")</f>
+        <v>365</v>
+      </c>
+      <c r="C159" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"D\")", "365");</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>30</v>
+      </c>
+      <c r="B160">
+        <f>DATEDIF("1/6/2019", "1/6/2020", "D")</f>
+        <v>366</v>
+      </c>
+      <c r="C160" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"D\")", "366");</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>30</v>
+      </c>
+      <c r="B161">
+        <f>DATEDIF("1/6/2020", "31/5/2021", "D")</f>
+        <v>364</v>
+      </c>
+      <c r="C161" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"D\")", "364");</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>30</v>
+      </c>
+      <c r="B162">
+        <f>DATEDIF("1/6/2020", "1/6/2021", "D")</f>
+        <v>365</v>
+      </c>
+      <c r="C162" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"D\")", "365");</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>30</v>
+      </c>
+      <c r="B163">
+        <f>DATEDIF("1/6/2019", "31/5/2020", "MD")</f>
+        <v>30</v>
+      </c>
+      <c r="C163" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"MD\")", "30");</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>30</v>
+      </c>
+      <c r="B164">
+        <f>DATEDIF("1/6/2019", "1/6/2020", "MD")</f>
+        <v>0</v>
+      </c>
+      <c r="C164" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"MD\")", "0");</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>30</v>
+      </c>
+      <c r="B165">
+        <f>DATEDIF("1/6/2020", "31/5/2021", "MD")</f>
+        <v>30</v>
+      </c>
+      <c r="C165" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"MD\")", "30");</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>30</v>
+      </c>
+      <c r="B166">
+        <f>DATEDIF("1/6/2020", "1/6/2021", "MD")</f>
+        <v>0</v>
+      </c>
+      <c r="C166" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"MD\")", "0");</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>30</v>
+      </c>
+      <c r="B167">
+        <f>DATEDIF("1/6/2019", "31/5/2020", "YM")</f>
+        <v>11</v>
+      </c>
+      <c r="C167" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"YM\")", "11");</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>30</v>
+      </c>
+      <c r="B168">
+        <f>DATEDIF("1/6/2019", "1/6/2020", "YM")</f>
+        <v>0</v>
+      </c>
+      <c r="C168" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"YM\")", "0");</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>30</v>
+      </c>
+      <c r="B169">
+        <f>DATEDIF("1/6/2020", "31/5/2021", "YM")</f>
+        <v>11</v>
+      </c>
+      <c r="C169" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"YM\")", "11");</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>30</v>
+      </c>
+      <c r="B170">
+        <f>DATEDIF("1/6/2020", "1/6/2021", "YM")</f>
+        <v>0</v>
+      </c>
+      <c r="C170" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"YM\")", "0");</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>30</v>
+      </c>
+      <c r="B171">
+        <f>DATEDIF("1/6/2019", "31/5/2020", "YD")</f>
+        <v>365</v>
+      </c>
+      <c r="C171" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"YD\")", "365");</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>30</v>
+      </c>
+      <c r="B172">
+        <f>DATEDIF("1/6/2019", "1/6/2020", "YD")</f>
+        <v>0</v>
+      </c>
+      <c r="C172" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"YD\")", "0");</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>30</v>
+      </c>
+      <c r="B173">
+        <f>DATEDIF("1/6/2020", "31/5/2021", "YD")</f>
+        <v>364</v>
+      </c>
+      <c r="C173" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"YD\")", "364");</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>30</v>
+      </c>
+      <c r="B174">
+        <f>DATEDIF("1/6/2020", "1/6/2021", "YD")</f>
+        <v>0</v>
+      </c>
+      <c r="C174" s="6" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"YD\")", "0");</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="7"/>
+      <c r="B175" s="7"/>
+      <c r="C175" s="8"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>32</v>
+      </c>
+      <c r="B176">
+        <f>HOUR(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C176" s="6" t="str">
+        <f t="shared" ref="C176:C181" ca="1" si="14">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B176),"""","\"""),";",","),""", """,IFERROR(B176,IF(ISNA(B176),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=HOUR(0)", "0");</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>32</v>
+      </c>
+      <c r="B177">
+        <f>HOUR(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C177" s="6" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>AssertExpression("=HOUR(1)", "0");</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>32</v>
+      </c>
+      <c r="B178">
+        <f>HOUR(0.75)</f>
+        <v>18</v>
+      </c>
+      <c r="C178" s="6" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>AssertExpression("=HOUR(0,75)", "18");</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>32</v>
+      </c>
+      <c r="B179">
+        <f>HOUR("18/7/2011 7:45")</f>
+        <v>7</v>
+      </c>
+      <c r="C179" s="6" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>AssertExpression("=HOUR(\"18/7/2011 7:45\")", "7");</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>32</v>
+      </c>
+      <c r="B180">
+        <f>HOUR("21/4/2012")</f>
+        <v>0</v>
+      </c>
+      <c r="C180" s="6" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>AssertExpression("=HOUR(\"21/4/2012\")", "0");</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>32</v>
+      </c>
+      <c r="B181" t="e">
+        <f>HOUR(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C181" s="6" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>AssertExpression("=HOUR(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>32</v>
+      </c>
+      <c r="B182">
+        <f>HOUR(0.74999)</f>
+        <v>17</v>
+      </c>
+      <c r="C182" s="6" t="str">
+        <f t="shared" ref="C182:C189" ca="1" si="15">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B182),"""","\"""),";",","),""", """,IFERROR(B182,IF(ISNA(B182),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=HOUR(0,74999)", "17");</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>32</v>
+      </c>
+      <c r="B183">
+        <f>HOUR(19/24-0.00001)</f>
+        <v>18</v>
+      </c>
+      <c r="C183" s="6" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>AssertExpression("=HOUR(19/24-0,00001)", "18");</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="7"/>
+      <c r="B184" s="7"/>
+      <c r="C184" s="8"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>33</v>
+      </c>
+      <c r="B185">
+        <f>MINUTE(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C185" s="6" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>AssertExpression("=MINUTE(0)", "0");</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>33</v>
+      </c>
+      <c r="B186">
+        <f>MINUTE(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C186" s="6" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>AssertExpression("=MINUTE(1)", "0");</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>33</v>
+      </c>
+      <c r="B187">
+        <f>MINUTE(0.75)</f>
+        <v>0</v>
+      </c>
+      <c r="C187" s="6" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>AssertExpression("=MINUTE(0,75)", "0");</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>33</v>
+      </c>
+      <c r="B188">
+        <f>MINUTE("12:45:00")</f>
+        <v>45</v>
+      </c>
+      <c r="C188" s="6" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>AssertExpression("=MINUTE(\"12:45:00\")", "45");</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>33</v>
+      </c>
+      <c r="B189" t="e">
+        <f>MINUTE(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C189" s="6" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>AssertExpression("=MINUTE(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>33</v>
+      </c>
+      <c r="B190">
+        <f>MINUTE(0.76)</f>
+        <v>14</v>
+      </c>
+      <c r="C190" s="6" t="str">
+        <f t="shared" ref="C190" ca="1" si="16">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B190),"""","\"""),";",","),""", """,IFERROR(B190,IF(ISNA(B190),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MINUTE(0,76)", "14");</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>33</v>
+      </c>
+      <c r="B191">
+        <f>MINUTE(0.765)</f>
+        <v>21</v>
+      </c>
+      <c r="C191" s="6" t="str">
+        <f t="shared" ref="C191" ca="1" si="17">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B191),"""","\"""),";",","),""", """,IFERROR(B191,IF(ISNA(B191),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MINUTE(0,765)", "21");</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>33</v>
+      </c>
+      <c r="B192">
+        <f>MINUTE(40000.765)</f>
+        <v>21</v>
+      </c>
+      <c r="C192" s="6" t="str">
+        <f t="shared" ref="C192:C214" ca="1" si="18">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B192),"""","\"""),";",","),""", """,IFERROR(B192,IF(ISNA(B192),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=MINUTE(40000,765)", "21");</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="7"/>
+      <c r="B193" s="7"/>
+      <c r="C193" s="8"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>34</v>
+      </c>
+      <c r="B194">
+        <f>SECOND(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C194" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(0)", "0");</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>34</v>
+      </c>
+      <c r="B195">
+        <f>SECOND(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C195" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(1)", "0");</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>34</v>
+      </c>
+      <c r="B196">
+        <f>SECOND(0.75)</f>
+        <v>0</v>
+      </c>
+      <c r="C196" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(0,75)", "0");</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>34</v>
+      </c>
+      <c r="B197">
+        <f>SECOND("12:45:32")</f>
+        <v>32</v>
+      </c>
+      <c r="C197" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(\"12:45:32\")", "32");</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>34</v>
+      </c>
+      <c r="B198" t="e">
+        <f>SECOND(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C198" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>34</v>
+      </c>
+      <c r="B199">
+        <f>SECOND(0.76)</f>
+        <v>24</v>
+      </c>
+      <c r="C199" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(0,76)", "24");</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>34</v>
+      </c>
+      <c r="B200">
+        <f>SECOND(0.765)</f>
+        <v>36</v>
+      </c>
+      <c r="C200" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(0,765)", "36");</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>34</v>
+      </c>
+      <c r="B201">
+        <f>SECOND(40000.765)</f>
+        <v>36</v>
+      </c>
+      <c r="C201" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=SECOND(40000,765)", "36");</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="7"/>
+      <c r="B202" s="7"/>
+      <c r="C202" s="8"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>35</v>
+      </c>
+      <c r="B203" t="e">
+        <f>DATEVALUE("")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C203" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=DATEVALUE(\"\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>35</v>
+      </c>
+      <c r="B204">
+        <f>DATEVALUE("22/8/2011")</f>
+        <v>40777</v>
+      </c>
+      <c r="C204" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=DATEVALUE(\"22/8/2011\")", "40777");</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>35</v>
+      </c>
+      <c r="B205">
+        <f>DATEVALUE("22-Απρ-2011")</f>
+        <v>40655</v>
+      </c>
+      <c r="C205" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=DATEVALUE(\"22-Απρ-2011\")", "40655");</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>35</v>
+      </c>
+      <c r="B206">
+        <f>DATEVALUE("23/2/2011")</f>
+        <v>40597</v>
+      </c>
+      <c r="C206" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=DATEVALUE(\"23/2/2011\")", "40597");</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>35</v>
+      </c>
+      <c r="B207">
+        <f>DATEVALUE("23-Ιουλ")</f>
+        <v>44035</v>
+      </c>
+      <c r="C207" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=DATEVALUE(\"23-Ιουλ\")", "44035");</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>35</v>
+      </c>
+      <c r="B208" t="e">
+        <f>DATEVALUE("22-Απλ-2011")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C208" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=DATEVALUE(\"22-Απλ-2011\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="7"/>
+      <c r="B209" s="7"/>
+      <c r="C209" s="8"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>36</v>
+      </c>
+      <c r="B210" t="e">
+        <f>TIMEVALUE("")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C210" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=TIMEVALUE(\"\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>36</v>
+      </c>
+      <c r="B211">
+        <f>TIMEVALUE("2:24 AM")</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="C211" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=TIMEVALUE(\"2:24 AM\")", "0,1");</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>36</v>
+      </c>
+      <c r="B212">
+        <f>TIMEVALUE("2:24 PM")</f>
+        <v>0.6</v>
+      </c>
+      <c r="C212" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=TIMEVALUE(\"2:24 PM\")", "0,6");</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>36</v>
+      </c>
+      <c r="B213">
+        <f>TIMEVALUE("22-Αυγ-2011 6:35 AM")</f>
+        <v>0.27430555555474712</v>
+      </c>
+      <c r="C213" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=TIMEVALUE(\"22-Αυγ-2011 6:35 AM\")", "0,274305555554747");</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>36</v>
+      </c>
+      <c r="B214">
+        <f>TIMEVALUE("2:24 μμ")</f>
+        <v>0.6</v>
+      </c>
+      <c r="C214" s="6" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>AssertExpression("=TIMEVALUE(\"2:24 μμ\")", "0,6");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for ISEVEN, ISODD, ISBLANK, ISERR, ISERROR, ISLOGICAL, ISNA, ISNONTEXT, ISTEXT, ISTEXT, N, TYPE functions
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="48">
   <si>
     <t>"A"</t>
   </si>
@@ -137,6 +137,39 @@
   </si>
   <si>
     <t>TIMEVALUE</t>
+  </si>
+  <si>
+    <t>ISBLANK</t>
+  </si>
+  <si>
+    <t>ISEVEN</t>
+  </si>
+  <si>
+    <t>ISERR</t>
+  </si>
+  <si>
+    <t>ISERROR</t>
+  </si>
+  <si>
+    <t>ISLOGICAL</t>
+  </si>
+  <si>
+    <t>ISNA</t>
+  </si>
+  <si>
+    <t>ISNUMBER</t>
+  </si>
+  <si>
+    <t>ISTEXT</t>
+  </si>
+  <si>
+    <t>ISNONTEXT</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1566,10 +1599,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,7 +3002,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="6" t="str">
-        <f t="shared" ref="C114:C120" ca="1" si="11">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B114),"""","\"""),";",","),""", """,IFERROR(B114,IF(ISNA(B114),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C114:C116" ca="1" si="11">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B114),"""","\"""),";",","),""", """,IFERROR(B114,IF(ISNA(B114),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=MONTH(1)", "1");</v>
       </c>
     </row>
@@ -3065,7 +3098,7 @@
         <v>1900</v>
       </c>
       <c r="C122" s="6" t="str">
-        <f t="shared" ref="C122:C128" ca="1" si="12">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B122),"""","\"""),";",","),""", """,IFERROR(B122,IF(ISNA(B122),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C122:C124" ca="1" si="12">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B122),"""","\"""),";",","),""", """,IFERROR(B122,IF(ISNA(B122),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=YEAR(1)", "1900");</v>
       </c>
     </row>
@@ -3161,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="C130" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B130),"""","\"""),";",","),""", """,IFERROR(B130,IF(ISNA(B130),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C130:C141" ca="1" si="13">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B130),"""","\"""),";",","),""", """,IFERROR(B130,IF(ISNA(B130),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=DAYS(0,0)", "0");</v>
       </c>
     </row>
@@ -3174,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="C131" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B131),"""","\"""),";",","),""", """,IFERROR(B131,IF(ISNA(B131),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(1,0)", "1");</v>
       </c>
     </row>
@@ -3187,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B132),"""","\"""),";",","),""", """,IFERROR(B132,IF(ISNA(B132),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(2,1)", "1");</v>
       </c>
     </row>
@@ -3200,7 +3233,7 @@
         <v>-1</v>
       </c>
       <c r="C133" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B133),"""","\"""),";",","),""", """,IFERROR(B133,IF(ISNA(B133),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(1,2)", "-1");</v>
       </c>
     </row>
@@ -3213,7 +3246,7 @@
         <v>2</v>
       </c>
       <c r="C134" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B134),"""","\"""),";",","),""", """,IFERROR(B134,IF(ISNA(B134),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(40002,999,40000,222)", "2");</v>
       </c>
     </row>
@@ -3226,7 +3259,7 @@
         <v>2</v>
       </c>
       <c r="C135" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B135),"""","\"""),";",","),""", """,IFERROR(B135,IF(ISNA(B135),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(\"20/4/2020\",\"18/4/2020\")", "2");</v>
       </c>
     </row>
@@ -3239,7 +3272,7 @@
         <v>7</v>
       </c>
       <c r="C136" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B136),"""","\"""),";",","),""", """,IFERROR(B136,IF(ISNA(B136),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(\"23/5/2020\",43967)", "7");</v>
       </c>
     </row>
@@ -3252,7 +3285,7 @@
         <v>-7</v>
       </c>
       <c r="C137" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B137),"""","\"""),";",","),""", """,IFERROR(B137,IF(ISNA(B137),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(43967,\"23/5/2020\")", "-7");</v>
       </c>
     </row>
@@ -3265,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="C138" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B138),"""","\"""),";",","),""", """,IFERROR(B138,IF(ISNA(B138),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(43967,99999,43967)", "0");</v>
       </c>
     </row>
@@ -3278,7 +3311,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B139),"""","\"""),";",","),""", """,IFERROR(B139,IF(ISNA(B139),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(43967,43967,99999)", "0");</v>
       </c>
     </row>
@@ -3291,7 +3324,7 @@
         <v>#NUM!</v>
       </c>
       <c r="C140" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B140),"""","\"""),";",","),""", """,IFERROR(B140,IF(ISNA(B140),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(43967,-1)", "#VALUE!");</v>
       </c>
     </row>
@@ -3304,7 +3337,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C141" s="6" t="str">
-        <f ca="1">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B141),"""","\"""),";",","),""", """,IFERROR(B141,IF(ISNA(B141),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ca="1" si="13"/>
         <v>AssertExpression("=DAYS(\"32/4/2020\",\"18/4/2020\")", "#VALUE!");</v>
       </c>
     </row>
@@ -3322,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="6" t="str">
-        <f t="shared" ref="C143:C174" ca="1" si="13">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B143),"""","\"""),";",","),""", """,IFERROR(B143,IF(ISNA(B143),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C143:C174" ca="1" si="14">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B143),"""","\"""),";",","),""", """,IFERROR(B143,IF(ISNA(B143),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"Y\")", "1");</v>
       </c>
     </row>
@@ -3335,7 +3368,7 @@
         <v>14</v>
       </c>
       <c r="C144" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"M\")", "14");</v>
       </c>
     </row>
@@ -3348,7 +3381,7 @@
         <v>440</v>
       </c>
       <c r="C145" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"D\")", "440");</v>
       </c>
     </row>
@@ -3361,7 +3394,7 @@
         <v>14</v>
       </c>
       <c r="C146" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"MD\")", "14");</v>
       </c>
     </row>
@@ -3374,7 +3407,7 @@
         <v>2</v>
       </c>
       <c r="C147" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"YM\")", "2");</v>
       </c>
     </row>
@@ -3387,7 +3420,7 @@
         <v>75</v>
       </c>
       <c r="C148" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2001\", \"15/8/2002\", \"YD\")", "75");</v>
       </c>
     </row>
@@ -3400,7 +3433,7 @@
         <v>#NUM!</v>
       </c>
       <c r="C149" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2003\", \"15/8/2002\", \"YD\")", "#VALUE!");</v>
       </c>
     </row>
@@ -3413,7 +3446,7 @@
         <v>2</v>
       </c>
       <c r="C150" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/1/2001\", \"1/1/2003\", \"Y\")", "2");</v>
       </c>
     </row>
@@ -3426,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="C151" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"Y\")", "0");</v>
       </c>
     </row>
@@ -3439,7 +3472,7 @@
         <v>1</v>
       </c>
       <c r="C152" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"Y\")", "1");</v>
       </c>
     </row>
@@ -3452,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="C153" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"Y\")", "0");</v>
       </c>
     </row>
@@ -3465,7 +3498,7 @@
         <v>1</v>
       </c>
       <c r="C154" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"Y\")", "1");</v>
       </c>
     </row>
@@ -3478,7 +3511,7 @@
         <v>11</v>
       </c>
       <c r="C155" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"M\")", "11");</v>
       </c>
     </row>
@@ -3491,7 +3524,7 @@
         <v>12</v>
       </c>
       <c r="C156" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"m\")", "12");</v>
       </c>
     </row>
@@ -3504,7 +3537,7 @@
         <v>11</v>
       </c>
       <c r="C157" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"m\")", "11");</v>
       </c>
     </row>
@@ -3517,7 +3550,7 @@
         <v>12</v>
       </c>
       <c r="C158" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"m\")", "12");</v>
       </c>
     </row>
@@ -3530,7 +3563,7 @@
         <v>365</v>
       </c>
       <c r="C159" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"D\")", "365");</v>
       </c>
     </row>
@@ -3543,7 +3576,7 @@
         <v>366</v>
       </c>
       <c r="C160" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"D\")", "366");</v>
       </c>
     </row>
@@ -3556,7 +3589,7 @@
         <v>364</v>
       </c>
       <c r="C161" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"D\")", "364");</v>
       </c>
     </row>
@@ -3569,7 +3602,7 @@
         <v>365</v>
       </c>
       <c r="C162" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"D\")", "365");</v>
       </c>
     </row>
@@ -3582,7 +3615,7 @@
         <v>30</v>
       </c>
       <c r="C163" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"MD\")", "30");</v>
       </c>
     </row>
@@ -3595,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="C164" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"MD\")", "0");</v>
       </c>
     </row>
@@ -3608,7 +3641,7 @@
         <v>30</v>
       </c>
       <c r="C165" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"MD\")", "30");</v>
       </c>
     </row>
@@ -3621,7 +3654,7 @@
         <v>0</v>
       </c>
       <c r="C166" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"MD\")", "0");</v>
       </c>
     </row>
@@ -3634,7 +3667,7 @@
         <v>11</v>
       </c>
       <c r="C167" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"YM\")", "11");</v>
       </c>
     </row>
@@ -3647,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="C168" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"YM\")", "0");</v>
       </c>
     </row>
@@ -3660,7 +3693,7 @@
         <v>11</v>
       </c>
       <c r="C169" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"YM\")", "11");</v>
       </c>
     </row>
@@ -3673,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="C170" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"YM\")", "0");</v>
       </c>
     </row>
@@ -3686,7 +3719,7 @@
         <v>365</v>
       </c>
       <c r="C171" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"31/5/2020\", \"YD\")", "365");</v>
       </c>
     </row>
@@ -3699,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="C172" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2019\", \"1/6/2020\", \"YD\")", "0");</v>
       </c>
     </row>
@@ -3712,7 +3745,7 @@
         <v>364</v>
       </c>
       <c r="C173" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"31/5/2021\", \"YD\")", "364");</v>
       </c>
     </row>
@@ -3725,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="C174" s="6" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>AssertExpression("=DATEDIF(\"1/6/2020\", \"1/6/2021\", \"YD\")", "0");</v>
       </c>
     </row>
@@ -3743,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="C176" s="6" t="str">
-        <f t="shared" ref="C176:C181" ca="1" si="14">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B176),"""","\"""),";",","),""", """,IFERROR(B176,IF(ISNA(B176),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C176:C181" ca="1" si="15">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B176),"""","\"""),";",","),""", """,IFERROR(B176,IF(ISNA(B176),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=HOUR(0)", "0");</v>
       </c>
     </row>
@@ -3756,7 +3789,7 @@
         <v>0</v>
       </c>
       <c r="C177" s="6" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>AssertExpression("=HOUR(1)", "0");</v>
       </c>
     </row>
@@ -3769,7 +3802,7 @@
         <v>18</v>
       </c>
       <c r="C178" s="6" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>AssertExpression("=HOUR(0,75)", "18");</v>
       </c>
     </row>
@@ -3782,7 +3815,7 @@
         <v>7</v>
       </c>
       <c r="C179" s="6" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>AssertExpression("=HOUR(\"18/7/2011 7:45\")", "7");</v>
       </c>
     </row>
@@ -3795,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="C180" s="6" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>AssertExpression("=HOUR(\"21/4/2012\")", "0");</v>
       </c>
     </row>
@@ -3808,7 +3841,7 @@
         <v>#NUM!</v>
       </c>
       <c r="C181" s="6" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>AssertExpression("=HOUR(-1)", "#VALUE!");</v>
       </c>
     </row>
@@ -3821,7 +3854,7 @@
         <v>17</v>
       </c>
       <c r="C182" s="6" t="str">
-        <f t="shared" ref="C182:C189" ca="1" si="15">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B182),"""","\"""),";",","),""", """,IFERROR(B182,IF(ISNA(B182),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C182:C189" ca="1" si="16">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B182),"""","\"""),";",","),""", """,IFERROR(B182,IF(ISNA(B182),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=HOUR(0,74999)", "17");</v>
       </c>
     </row>
@@ -3834,7 +3867,7 @@
         <v>18</v>
       </c>
       <c r="C183" s="6" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>AssertExpression("=HOUR(19/24-0,00001)", "18");</v>
       </c>
     </row>
@@ -3852,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="C185" s="6" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>AssertExpression("=MINUTE(0)", "0");</v>
       </c>
     </row>
@@ -3865,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="C186" s="6" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>AssertExpression("=MINUTE(1)", "0");</v>
       </c>
     </row>
@@ -3878,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="C187" s="6" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>AssertExpression("=MINUTE(0,75)", "0");</v>
       </c>
     </row>
@@ -3891,7 +3924,7 @@
         <v>45</v>
       </c>
       <c r="C188" s="6" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>AssertExpression("=MINUTE(\"12:45:00\")", "45");</v>
       </c>
     </row>
@@ -3904,7 +3937,7 @@
         <v>#NUM!</v>
       </c>
       <c r="C189" s="6" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>AssertExpression("=MINUTE(-1)", "#VALUE!");</v>
       </c>
     </row>
@@ -3917,7 +3950,7 @@
         <v>14</v>
       </c>
       <c r="C190" s="6" t="str">
-        <f t="shared" ref="C190" ca="1" si="16">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B190),"""","\"""),";",","),""", """,IFERROR(B190,IF(ISNA(B190),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C190" ca="1" si="17">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B190),"""","\"""),";",","),""", """,IFERROR(B190,IF(ISNA(B190),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=MINUTE(0,76)", "14");</v>
       </c>
     </row>
@@ -3930,7 +3963,7 @@
         <v>21</v>
       </c>
       <c r="C191" s="6" t="str">
-        <f t="shared" ref="C191" ca="1" si="17">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B191),"""","\"""),";",","),""", """,IFERROR(B191,IF(ISNA(B191),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C191" ca="1" si="18">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B191),"""","\"""),";",","),""", """,IFERROR(B191,IF(ISNA(B191),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=MINUTE(0,765)", "21");</v>
       </c>
     </row>
@@ -3943,7 +3976,7 @@
         <v>21</v>
       </c>
       <c r="C192" s="6" t="str">
-        <f t="shared" ref="C192:C214" ca="1" si="18">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B192),"""","\"""),";",","),""", """,IFERROR(B192,IF(ISNA(B192),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C192:C243" ca="1" si="19">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B192),"""","\"""),";",","),""", """,IFERROR(B192,IF(ISNA(B192),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=MINUTE(40000,765)", "21");</v>
       </c>
     </row>
@@ -3961,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="C194" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(0)", "0");</v>
       </c>
     </row>
@@ -3974,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="C195" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(1)", "0");</v>
       </c>
     </row>
@@ -3987,7 +4020,7 @@
         <v>0</v>
       </c>
       <c r="C196" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(0,75)", "0");</v>
       </c>
     </row>
@@ -4000,7 +4033,7 @@
         <v>32</v>
       </c>
       <c r="C197" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(\"12:45:32\")", "32");</v>
       </c>
     </row>
@@ -4013,7 +4046,7 @@
         <v>#NUM!</v>
       </c>
       <c r="C198" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(-1)", "#VALUE!");</v>
       </c>
     </row>
@@ -4026,7 +4059,7 @@
         <v>24</v>
       </c>
       <c r="C199" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(0,76)", "24");</v>
       </c>
     </row>
@@ -4039,7 +4072,7 @@
         <v>36</v>
       </c>
       <c r="C200" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(0,765)", "36");</v>
       </c>
     </row>
@@ -4052,7 +4085,7 @@
         <v>36</v>
       </c>
       <c r="C201" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=SECOND(40000,765)", "36");</v>
       </c>
     </row>
@@ -4070,7 +4103,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C203" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=DATEVALUE(\"\")", "#VALUE!");</v>
       </c>
     </row>
@@ -4083,7 +4116,7 @@
         <v>40777</v>
       </c>
       <c r="C204" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=DATEVALUE(\"22/8/2011\")", "40777");</v>
       </c>
     </row>
@@ -4096,7 +4129,7 @@
         <v>40655</v>
       </c>
       <c r="C205" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=DATEVALUE(\"22-Απρ-2011\")", "40655");</v>
       </c>
     </row>
@@ -4109,7 +4142,7 @@
         <v>40597</v>
       </c>
       <c r="C206" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=DATEVALUE(\"23/2/2011\")", "40597");</v>
       </c>
     </row>
@@ -4122,7 +4155,7 @@
         <v>44035</v>
       </c>
       <c r="C207" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=DATEVALUE(\"23-Ιουλ\")", "44035");</v>
       </c>
     </row>
@@ -4135,7 +4168,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C208" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=DATEVALUE(\"22-Απλ-2011\")", "#VALUE!");</v>
       </c>
     </row>
@@ -4153,7 +4186,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C210" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=TIMEVALUE(\"\")", "#VALUE!");</v>
       </c>
     </row>
@@ -4166,7 +4199,7 @@
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="C211" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=TIMEVALUE(\"2:24 AM\")", "0,1");</v>
       </c>
     </row>
@@ -4179,7 +4212,7 @@
         <v>0.6</v>
       </c>
       <c r="C212" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=TIMEVALUE(\"2:24 PM\")", "0,6");</v>
       </c>
     </row>
@@ -4192,7 +4225,7 @@
         <v>0.27430555555474712</v>
       </c>
       <c r="C213" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=TIMEVALUE(\"22-Αυγ-2011 6:35 AM\")", "0,274305555554747");</v>
       </c>
     </row>
@@ -4205,9 +4238,1239 @@
         <v>0.6</v>
       </c>
       <c r="C214" s="6" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>AssertExpression("=TIMEVALUE(\"2:24 μμ\")", "0,6");</v>
       </c>
+    </row>
+    <row r="215" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="7"/>
+      <c r="B215" s="7"/>
+      <c r="C215" s="8"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>38</v>
+      </c>
+      <c r="B216" t="b">
+        <f>ISEVEN(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C216" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(0)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>38</v>
+      </c>
+      <c r="B217" t="b">
+        <f>ISEVEN(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C217" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(1)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>38</v>
+      </c>
+      <c r="B218" t="b">
+        <f>ISEVEN(2)</f>
+        <v>1</v>
+      </c>
+      <c r="C218" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(2)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>38</v>
+      </c>
+      <c r="B219" t="b">
+        <f>ISEVEN(-1)</f>
+        <v>0</v>
+      </c>
+      <c r="C219" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(-1)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>38</v>
+      </c>
+      <c r="B220" t="b">
+        <f>ISEVEN(1.5)</f>
+        <v>0</v>
+      </c>
+      <c r="C220" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(1,5)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>38</v>
+      </c>
+      <c r="B221" t="b">
+        <f>ISEVEN(2.5)</f>
+        <v>1</v>
+      </c>
+      <c r="C221" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(2,5)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>38</v>
+      </c>
+      <c r="B222" t="b">
+        <f>ISEVEN(-2.9)</f>
+        <v>1</v>
+      </c>
+      <c r="C222" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(-2,9)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>38</v>
+      </c>
+      <c r="B223" t="b">
+        <f>ISEVEN("10")</f>
+        <v>1</v>
+      </c>
+      <c r="C223" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(\"10\")", "TRUE");</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>38</v>
+      </c>
+      <c r="B224" t="e">
+        <f>ISEVEN("10A")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C224" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(\"10A\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>38</v>
+      </c>
+      <c r="B225" t="e">
+        <f>ISEVEN(NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C225" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(NA())", "#N/A");</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>38</v>
+      </c>
+      <c r="B226" t="b">
+        <f>ISEVEN(DATE(2020,5,16))</f>
+        <v>0</v>
+      </c>
+      <c r="C226" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(DATE(2020,5,16))", "FALSE");</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>38</v>
+      </c>
+      <c r="B227" t="e">
+        <f>ISEVEN(TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C227" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(TRUE)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>38</v>
+      </c>
+      <c r="B228" t="e">
+        <f>ISEVEN(FALSE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C228" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISEVEN(FALSE)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="7"/>
+      <c r="B229" s="7"/>
+      <c r="C229" s="8"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>37</v>
+      </c>
+      <c r="B230" t="b">
+        <f>ISBLANK("")</f>
+        <v>0</v>
+      </c>
+      <c r="C230" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(\"\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>37</v>
+      </c>
+      <c r="B231" t="b">
+        <f>ISBLANK(NA())</f>
+        <v>0</v>
+      </c>
+      <c r="C231" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(NA())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>37</v>
+      </c>
+      <c r="B232" t="b">
+        <f>ISBLANK(D232)</f>
+        <v>1</v>
+      </c>
+      <c r="C232" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(D232)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>37</v>
+      </c>
+      <c r="B233" t="b">
+        <f>ISBLANK(D233:D234)</f>
+        <v>1</v>
+      </c>
+      <c r="C233" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(D233:D234)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>37</v>
+      </c>
+      <c r="B234" t="b">
+        <f>ISBLANK(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C234" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>37</v>
+      </c>
+      <c r="B235" t="b">
+        <f>ISBLANK(TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="C235" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(TRUE)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>37</v>
+      </c>
+      <c r="B236" t="b">
+        <f ca="1">ISBLANK(NOW())</f>
+        <v>0</v>
+      </c>
+      <c r="C236" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISBLANK(NOW())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="7"/>
+      <c r="B237" s="7"/>
+      <c r="C237" s="8"/>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>39</v>
+      </c>
+      <c r="B238" t="b">
+        <f>ISERR("")</f>
+        <v>0</v>
+      </c>
+      <c r="C238" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISERR(\"\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>39</v>
+      </c>
+      <c r="B239" t="b">
+        <f>ISERR(NA())</f>
+        <v>0</v>
+      </c>
+      <c r="C239" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISERR(NA())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>39</v>
+      </c>
+      <c r="B240" t="b">
+        <f>ISERR(1/0)</f>
+        <v>1</v>
+      </c>
+      <c r="C240" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISERR(1/0)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>39</v>
+      </c>
+      <c r="B241" t="b">
+        <f>ISERR(ISEVEN(TRUE))</f>
+        <v>1</v>
+      </c>
+      <c r="C241" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISERR(ISEVEN(TRUE))", "TRUE");</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>39</v>
+      </c>
+      <c r="B242" t="b">
+        <f>ISERR(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C242" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISERR(0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>39</v>
+      </c>
+      <c r="B243" t="b">
+        <f>ISERR(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C243" s="6" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>AssertExpression("=ISERR(0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="7"/>
+      <c r="B244" s="7"/>
+      <c r="C244" s="8"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>40</v>
+      </c>
+      <c r="B245" t="b">
+        <f>ISERROR("")</f>
+        <v>0</v>
+      </c>
+      <c r="C245" s="6" t="str">
+        <f t="shared" ref="C245:C272" ca="1" si="20">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B245),"""","\"""),";",","),""", """,IFERROR(B245,IF(ISNA(B245),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=ISERROR(\"\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>40</v>
+      </c>
+      <c r="B246" t="b">
+        <f>ISERROR(NA())</f>
+        <v>1</v>
+      </c>
+      <c r="C246" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISERROR(NA())", "TRUE");</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>40</v>
+      </c>
+      <c r="B247" t="b">
+        <f>ISERROR(1/0)</f>
+        <v>1</v>
+      </c>
+      <c r="C247" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISERROR(1/0)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>40</v>
+      </c>
+      <c r="B248" t="b">
+        <f>ISERROR(ISEVEN(TRUE))</f>
+        <v>1</v>
+      </c>
+      <c r="C248" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISERROR(ISEVEN(TRUE))", "TRUE");</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>40</v>
+      </c>
+      <c r="B249" t="b">
+        <f>ISERROR(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C249" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISERROR(0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>40</v>
+      </c>
+      <c r="B250" t="b">
+        <f>ISERROR(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C250" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISERROR(0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="7"/>
+      <c r="B251" s="7"/>
+      <c r="C251" s="8"/>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>41</v>
+      </c>
+      <c r="B252" t="b">
+        <f>ISLOGICAL(TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="C252" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(TRUE)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>41</v>
+      </c>
+      <c r="B253" t="b">
+        <f>ISLOGICAL(FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="C253" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(FALSE)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>41</v>
+      </c>
+      <c r="B254" t="b">
+        <f>ISLOGICAL(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C254" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(1)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>41</v>
+      </c>
+      <c r="B255" t="b">
+        <f>ISLOGICAL("abc")</f>
+        <v>0</v>
+      </c>
+      <c r="C255" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(\"abc\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>41</v>
+      </c>
+      <c r="B256" t="b">
+        <f>ISLOGICAL(1/0)</f>
+        <v>0</v>
+      </c>
+      <c r="C256" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(1/0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>41</v>
+      </c>
+      <c r="B257" t="b">
+        <f>ISLOGICAL(NA())</f>
+        <v>0</v>
+      </c>
+      <c r="C257" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(NA())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>41</v>
+      </c>
+      <c r="B258" t="b">
+        <f>ISLOGICAL(ISERR(123))</f>
+        <v>1</v>
+      </c>
+      <c r="C258" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(ISERR(123))", "TRUE");</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>41</v>
+      </c>
+      <c r="B259" t="b">
+        <f>ISLOGICAL(10/"a")</f>
+        <v>0</v>
+      </c>
+      <c r="C259" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISLOGICAL(10/\"a\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="7"/>
+      <c r="B260" s="7"/>
+      <c r="C260" s="8"/>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>42</v>
+      </c>
+      <c r="B261" t="b">
+        <f>ISNA(NA())</f>
+        <v>1</v>
+      </c>
+      <c r="C261" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNA(NA())", "TRUE");</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>42</v>
+      </c>
+      <c r="B262" t="b">
+        <f>ISNA(1/0)</f>
+        <v>0</v>
+      </c>
+      <c r="C262" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNA(1/0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>42</v>
+      </c>
+      <c r="B263" t="b">
+        <f>ISNA(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C263" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNA(1)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>42</v>
+      </c>
+      <c r="B264" t="b">
+        <f>ISNA(FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C264" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNA(FALSE)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>42</v>
+      </c>
+      <c r="B265" t="b">
+        <f>ISNA(10/"a")</f>
+        <v>0</v>
+      </c>
+      <c r="C265" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNA(10/\"a\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="7"/>
+      <c r="B266" s="7"/>
+      <c r="C266" s="8"/>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>43</v>
+      </c>
+      <c r="B267" t="b">
+        <f>ISNUMBER(1)</f>
+        <v>1</v>
+      </c>
+      <c r="C267" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNUMBER(1)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>43</v>
+      </c>
+      <c r="B268" t="b">
+        <f>ISNUMBER(10.1)</f>
+        <v>1</v>
+      </c>
+      <c r="C268" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNUMBER(10,1)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>43</v>
+      </c>
+      <c r="B269" t="b">
+        <f>ISNUMBER("10")</f>
+        <v>0</v>
+      </c>
+      <c r="C269" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNUMBER(\"10\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>43</v>
+      </c>
+      <c r="B270" t="b">
+        <f>ISNUMBER(TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="C270" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNUMBER(TRUE)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>43</v>
+      </c>
+      <c r="B271" t="b">
+        <f>ISNUMBER(NA())</f>
+        <v>0</v>
+      </c>
+      <c r="C271" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNUMBER(NA())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>43</v>
+      </c>
+      <c r="B272" t="b">
+        <f>ISNUMBER(1/0)</f>
+        <v>0</v>
+      </c>
+      <c r="C272" s="6" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>AssertExpression("=ISNUMBER(1/0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>43</v>
+      </c>
+      <c r="B273" t="b">
+        <f ca="1">ISNUMBER(NOW())</f>
+        <v>1</v>
+      </c>
+      <c r="C273" s="6" t="str">
+        <f t="shared" ref="C273" ca="1" si="21">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B273),"""","\"""),";",","),""", """,IFERROR(B273,IF(ISNA(B273),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=ISNUMBER(NOW())", "TRUE");</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>43</v>
+      </c>
+      <c r="B274" t="b">
+        <f>ISNUMBER(TIME(10,10,10))</f>
+        <v>1</v>
+      </c>
+      <c r="C274" s="6" t="str">
+        <f t="shared" ref="C274:C315" ca="1" si="22">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B274),"""","\"""),";",","),""", """,IFERROR(B274,IF(ISNA(B274),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=ISNUMBER(TIME(10,10,10))", "TRUE");</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="7"/>
+      <c r="B275" s="7"/>
+      <c r="C275" s="8"/>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>44</v>
+      </c>
+      <c r="B276" t="b">
+        <f>ISTEXT("")</f>
+        <v>1</v>
+      </c>
+      <c r="C276" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(\"\")", "TRUE");</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>44</v>
+      </c>
+      <c r="B277" t="b">
+        <f>ISTEXT("10")</f>
+        <v>1</v>
+      </c>
+      <c r="C277" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(\"10\")", "TRUE");</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>44</v>
+      </c>
+      <c r="B278" t="b">
+        <f>ISTEXT(7 &amp; "A")</f>
+        <v>1</v>
+      </c>
+      <c r="C278" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(7 &amp; \"A\")", "TRUE");</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>44</v>
+      </c>
+      <c r="B279" t="b">
+        <f>ISTEXT(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C279" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(1)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>44</v>
+      </c>
+      <c r="B280" t="b">
+        <f>ISTEXT(TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="C280" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(TRUE)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>44</v>
+      </c>
+      <c r="B281" t="b">
+        <f>ISTEXT(NA())</f>
+        <v>0</v>
+      </c>
+      <c r="C281" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(NA())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>44</v>
+      </c>
+      <c r="B282" t="b">
+        <f>ISTEXT(1/0)</f>
+        <v>0</v>
+      </c>
+      <c r="C282" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(1/0)", "FALSE");</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>44</v>
+      </c>
+      <c r="B283" t="b">
+        <f ca="1">ISTEXT(NOW())</f>
+        <v>0</v>
+      </c>
+      <c r="C283" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISTEXT(NOW())", "FALSE");</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="7"/>
+      <c r="B284" s="7"/>
+      <c r="C284" s="8"/>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>45</v>
+      </c>
+      <c r="B285" t="b">
+        <f>ISNONTEXT("")</f>
+        <v>0</v>
+      </c>
+      <c r="C285" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(\"\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>45</v>
+      </c>
+      <c r="B286" t="b">
+        <f>ISNONTEXT("10")</f>
+        <v>0</v>
+      </c>
+      <c r="C286" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(\"10\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>45</v>
+      </c>
+      <c r="B287" t="b">
+        <f>ISNONTEXT(7 &amp; "A")</f>
+        <v>0</v>
+      </c>
+      <c r="C287" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(7 &amp; \"A\")", "FALSE");</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>45</v>
+      </c>
+      <c r="B288" t="b">
+        <f>ISNONTEXT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="C288" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(1)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>45</v>
+      </c>
+      <c r="B289" t="b">
+        <f>ISNONTEXT(TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="C289" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(TRUE)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>45</v>
+      </c>
+      <c r="B290" t="b">
+        <f>ISNONTEXT(NA())</f>
+        <v>1</v>
+      </c>
+      <c r="C290" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(NA())", "TRUE");</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>45</v>
+      </c>
+      <c r="B291" t="b">
+        <f>ISNONTEXT(1/0)</f>
+        <v>1</v>
+      </c>
+      <c r="C291" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(1/0)", "TRUE");</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>45</v>
+      </c>
+      <c r="B292" t="b">
+        <f ca="1">ISNONTEXT(NOW())</f>
+        <v>1</v>
+      </c>
+      <c r="C292" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ISNONTEXT(NOW())", "TRUE");</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="7"/>
+      <c r="B293" s="7"/>
+      <c r="C293" s="8"/>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>46</v>
+      </c>
+      <c r="B294">
+        <f>TYPE(1)</f>
+        <v>1</v>
+      </c>
+      <c r="C294" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(1)", "1");</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>46</v>
+      </c>
+      <c r="B295">
+        <f>TYPE(FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="C295" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(FALSE)", "4");</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>46</v>
+      </c>
+      <c r="B296">
+        <f>TYPE(1.23)</f>
+        <v>1</v>
+      </c>
+      <c r="C296" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(1,23)", "1");</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>46</v>
+      </c>
+      <c r="B297">
+        <f ca="1">TYPE(NOW())</f>
+        <v>1</v>
+      </c>
+      <c r="C297" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(NOW())", "1");</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>46</v>
+      </c>
+      <c r="B298">
+        <f>TYPE("")</f>
+        <v>2</v>
+      </c>
+      <c r="C298" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(\"\")", "2");</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>46</v>
+      </c>
+      <c r="B299">
+        <f>TYPE(NA())</f>
+        <v>16</v>
+      </c>
+      <c r="C299" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(NA())", "16");</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>46</v>
+      </c>
+      <c r="B300">
+        <f>TYPE(1/0)</f>
+        <v>16</v>
+      </c>
+      <c r="C300" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(1/0)", "16");</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>46</v>
+      </c>
+      <c r="B301">
+        <f>TYPE(2+"a")</f>
+        <v>16</v>
+      </c>
+      <c r="C301" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE(2+\"a\")", "16");</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>46</v>
+      </c>
+      <c r="B302">
+        <f>TYPE({1.2;3.4})</f>
+        <v>64</v>
+      </c>
+      <c r="C302" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=TYPE({1,2,3,4})", "64");</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="7"/>
+      <c r="B303" s="7"/>
+      <c r="C303" s="8"/>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>47</v>
+      </c>
+      <c r="B304">
+        <f>N(2)</f>
+        <v>2</v>
+      </c>
+      <c r="C304" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(2)", "2");</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>47</v>
+      </c>
+      <c r="B305">
+        <f>N(3.14)</f>
+        <v>3.14</v>
+      </c>
+      <c r="C305" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(3,14)", "3,14");</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>47</v>
+      </c>
+      <c r="B306">
+        <f>N(DATE(2020,5,16) + TIME(11,32,23))</f>
+        <v>43967.480821759258</v>
+      </c>
+      <c r="C306" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(DATE(2020,5,16) + TIME(11,32,23))", "43967,4808217593");</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>47</v>
+      </c>
+      <c r="B307">
+        <f>N("12/3/2020")</f>
+        <v>0</v>
+      </c>
+      <c r="C307" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(\"12/3/2020\")", "0");</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>47</v>
+      </c>
+      <c r="B308">
+        <f>N(TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="C308" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(TRUE)", "1");</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>47</v>
+      </c>
+      <c r="B309">
+        <f>N(FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C309" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(FALSE)", "0");</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>47</v>
+      </c>
+      <c r="B310">
+        <f>N("1")</f>
+        <v>0</v>
+      </c>
+      <c r="C310" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(\"1\")", "0");</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>47</v>
+      </c>
+      <c r="B311" t="e">
+        <f>N(NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C311" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(NA())", "#N/A");</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>47</v>
+      </c>
+      <c r="B312" t="e">
+        <f>N(1/0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C312" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(1/0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>47</v>
+      </c>
+      <c r="B313" t="e">
+        <f>N(1+"a")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C313" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(1+\"a\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>47</v>
+      </c>
+      <c r="B314">
+        <f>N("")</f>
+        <v>0</v>
+      </c>
+      <c r="C314" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(\"\")", "0");</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>47</v>
+      </c>
+      <c r="B315">
+        <f>N("10")</f>
+        <v>0</v>
+      </c>
+      <c r="C315" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=N(\"10\")", "0");</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="7"/>
+      <c r="B316" s="7"/>
+      <c r="C316" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4218,10 +5481,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:H18"/>
+  <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4347,6 +5610,10 @@
         <f>TIME(B10,B11,B12)</f>
         <v>0.42526620370370366</v>
       </c>
+      <c r="E10" t="str">
+        <f>D10 &amp; " aaa"</f>
+        <v>0,425266203703704 aaa</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -4385,7 +5652,7 @@
         <v>43901</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
@@ -4393,12 +5660,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B18">
         <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="e">
+        <f>NA() &amp;(1/0)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for ACOS, ACOSH, ACOT, ACOTH, ASIN, ASINH, ATAN, ATAN2, ATANH, COS, COSH, COT, COTH, CSC, CSCH, SEC, SECH, SIN, SINH, TAN, TANH
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="66">
   <si>
     <t>"A"</t>
   </si>
@@ -170,6 +170,60 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>ACOS</t>
+  </si>
+  <si>
+    <t>ACOSH</t>
+  </si>
+  <si>
+    <t>ASIN</t>
+  </si>
+  <si>
+    <t>ASINH</t>
+  </si>
+  <si>
+    <t>ACOT</t>
+  </si>
+  <si>
+    <t>ACOTH</t>
+  </si>
+  <si>
+    <t>ATAN</t>
+  </si>
+  <si>
+    <t>ATAN2</t>
+  </si>
+  <si>
+    <t>ATANH</t>
+  </si>
+  <si>
+    <t>COS</t>
+  </si>
+  <si>
+    <t>COSH</t>
+  </si>
+  <si>
+    <t>COT</t>
+  </si>
+  <si>
+    <t>COTH</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>CSCH</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>SECH</t>
   </si>
 </sst>
 </file>
@@ -1599,10 +1653,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C316"/>
+  <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
-      <selection activeCell="C311" sqref="C311"/>
+    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
+      <selection activeCell="C428" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4962,7 +5016,7 @@
         <v>1</v>
       </c>
       <c r="C274" s="6" t="str">
-        <f t="shared" ref="C274:C315" ca="1" si="22">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B274),"""","\"""),";",","),""", """,IFERROR(B274,IF(ISNA(B274),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C274:C337" ca="1" si="22">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B274),"""","\"""),";",","),""", """,IFERROR(B274,IF(ISNA(B274),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=ISNUMBER(TIME(10,10,10))", "TRUE");</v>
       </c>
     </row>
@@ -5471,6 +5525,1409 @@
       <c r="A316" s="7"/>
       <c r="B316" s="7"/>
       <c r="C316" s="8"/>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>48</v>
+      </c>
+      <c r="B317">
+        <f>ABS(2.5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="C317" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(2,5)", "2,5");</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>48</v>
+      </c>
+      <c r="B318">
+        <f>ABS(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C318" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(0)", "0");</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>48</v>
+      </c>
+      <c r="B319">
+        <f>ABS(-2.5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="C319" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(-2,5)", "2,5");</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>48</v>
+      </c>
+      <c r="B320">
+        <f>ABS(-TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="C320" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(-TRUE)", "1");</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>48</v>
+      </c>
+      <c r="B321">
+        <f>ABS(-TIME(23,59,59))</f>
+        <v>0.99998842592592585</v>
+      </c>
+      <c r="C321" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(-TIME(23,59,59))", "0,999988425925926");</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>48</v>
+      </c>
+      <c r="B322">
+        <f>ABS("-12")</f>
+        <v>12</v>
+      </c>
+      <c r="C322" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(\"-12\")", "12");</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>48</v>
+      </c>
+      <c r="B323" t="e">
+        <f>ABS("abc")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C323" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ABS(\"abc\")", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="7"/>
+      <c r="B324" s="7"/>
+      <c r="C324" s="8"/>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>49</v>
+      </c>
+      <c r="B325">
+        <f>ACOS(0)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C325" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOS(0)", "1,5707963267949");</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>49</v>
+      </c>
+      <c r="B326">
+        <f>ACOS(-1)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="C326" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOS(-1)", "3,14159265358979");</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>49</v>
+      </c>
+      <c r="B327">
+        <f>ACOS(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C327" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOS(1)", "0");</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>49</v>
+      </c>
+      <c r="B328" t="e">
+        <f>ACOS(1.5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C328" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOS(1,5)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>49</v>
+      </c>
+      <c r="B329" t="e">
+        <f>ACOS(-1.5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C329" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOS(-1,5)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="7"/>
+      <c r="B330" s="7"/>
+      <c r="C330" s="8"/>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>50</v>
+      </c>
+      <c r="B331" t="e">
+        <f>ACOSH(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C331" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOSH(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>50</v>
+      </c>
+      <c r="B332" t="e">
+        <f>ACOSH(0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C332" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOSH(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>50</v>
+      </c>
+      <c r="B333">
+        <f>ACOSH(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C333" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOSH(1)", "0");</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>50</v>
+      </c>
+      <c r="B334">
+        <f>ACOSH(1111)</f>
+        <v>7.7061627676590074</v>
+      </c>
+      <c r="C334" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOSH(1111)", "7,70616276765901");</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>50</v>
+      </c>
+      <c r="B335">
+        <f>ACOSH(1111111.111)</f>
+        <v>14.614018254081843</v>
+      </c>
+      <c r="C335" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ACOSH(1111111,111)", "14,6140182540818");</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="7"/>
+      <c r="B336" s="7"/>
+      <c r="C336" s="8"/>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>51</v>
+      </c>
+      <c r="B337">
+        <f>ASIN(-1)</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="C337" s="6" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>AssertExpression("=ASIN(-1)", "-1,5707963267949");</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>51</v>
+      </c>
+      <c r="B338">
+        <f>ASIN(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C338" s="6" t="str">
+        <f t="shared" ref="C338:C341" ca="1" si="23">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B338),"""","\"""),";",","),""", """,IFERROR(B338,IF(ISNA(B338),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=ASIN(0)", "0");</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>51</v>
+      </c>
+      <c r="B339">
+        <f>ASIN(1)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C339" s="6" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v>AssertExpression("=ASIN(1)", "1,5707963267949");</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>51</v>
+      </c>
+      <c r="B340" t="e">
+        <f>ASIN(-1.1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C340" s="6" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v>AssertExpression("=ASIN(-1,1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>51</v>
+      </c>
+      <c r="B341" t="e">
+        <f>ASIN(1.1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C341" s="6" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v>AssertExpression("=ASIN(1,1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="7"/>
+      <c r="B342" s="7"/>
+      <c r="C342" s="8"/>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>52</v>
+      </c>
+      <c r="B343">
+        <f>ASINH(-1)</f>
+        <v>-0.88137358701954294</v>
+      </c>
+      <c r="C343" s="6" t="str">
+        <f t="shared" ref="C343:C406" ca="1" si="24">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B343),"""","\"""),";",","),""", """,IFERROR(B343,IF(ISNA(B343),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=ASINH(-1)", "-0,881373587019543");</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>52</v>
+      </c>
+      <c r="B344">
+        <f>ASINH(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C344" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ASINH(0)", "0");</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>52</v>
+      </c>
+      <c r="B345">
+        <f>ASINH(1)</f>
+        <v>0.88137358701954294</v>
+      </c>
+      <c r="C345" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ASINH(1)", "0,881373587019543");</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>52</v>
+      </c>
+      <c r="B346">
+        <f>ASINH(1111)</f>
+        <v>7.7061631727400197</v>
+      </c>
+      <c r="C346" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ASINH(1111)", "7,70616317274002");</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>52</v>
+      </c>
+      <c r="B347">
+        <f>ASINH(1111111.111)</f>
+        <v>14.614018254082248</v>
+      </c>
+      <c r="C347" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ASINH(1111111,111)", "14,6140182540822");</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="7"/>
+      <c r="B348" s="7"/>
+      <c r="C348" s="8"/>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>53</v>
+      </c>
+      <c r="B349">
+        <f>_xlfn.ACOT(0)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C349" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOT(0)", "1,5707963267949");</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>53</v>
+      </c>
+      <c r="B350">
+        <f>_xlfn.ACOT(-1)</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="C350" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOT(-1)", "2,35619449019234");</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>53</v>
+      </c>
+      <c r="B351">
+        <f>_xlfn.ACOT(-2)</f>
+        <v>2.677945044588987</v>
+      </c>
+      <c r="C351" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOT(-2)", "2,67794504458899");</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>53</v>
+      </c>
+      <c r="B352">
+        <f>_xlfn.ACOT(1)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C352" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOT(1)", "0,785398163397448");</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>53</v>
+      </c>
+      <c r="B353">
+        <f>_xlfn.ACOT(2)</f>
+        <v>0.46364760900080609</v>
+      </c>
+      <c r="C353" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOT(2)", "0,463647609000806");</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="7"/>
+      <c r="B354" s="7"/>
+      <c r="C354" s="8"/>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>54</v>
+      </c>
+      <c r="B355" t="e">
+        <f>_xlfn.ACOTH(0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C355" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>54</v>
+      </c>
+      <c r="B356" t="e">
+        <f>_xlfn.ACOTH(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C356" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>54</v>
+      </c>
+      <c r="B357">
+        <f>_xlfn.ACOTH(-2)</f>
+        <v>-0.54930614433405489</v>
+      </c>
+      <c r="C357" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(-2)", "-0,549306144334055");</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>54</v>
+      </c>
+      <c r="B358" t="e">
+        <f>_xlfn.ACOTH(1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C358" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>54</v>
+      </c>
+      <c r="B359">
+        <f>_xlfn.ACOTH(2)</f>
+        <v>0.54930614433405489</v>
+      </c>
+      <c r="C359" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(2)", "0,549306144334055");</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>54</v>
+      </c>
+      <c r="B360">
+        <f>_xlfn.ACOTH(1112)</f>
+        <v>8.9928081795741786E-4</v>
+      </c>
+      <c r="C360" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(1112)", "0,000899280817957418");</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>54</v>
+      </c>
+      <c r="B361">
+        <f>_xlfn.ACOTH(3)</f>
+        <v>0.34657359027997264</v>
+      </c>
+      <c r="C361" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(3)", "0,346573590279973");</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>54</v>
+      </c>
+      <c r="B362">
+        <f>_xlfn.ACOTH(-PI())</f>
+        <v>-0.32976531495669914</v>
+      </c>
+      <c r="C362" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ACOTH(-PI())", "-0,329765314956699");</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="7"/>
+      <c r="B363" s="7"/>
+      <c r="C363" s="8"/>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>55</v>
+      </c>
+      <c r="B364">
+        <f>ATAN(-444)</f>
+        <v>-1.5685440783509212</v>
+      </c>
+      <c r="C364" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN(-444)", "-1,56854407835092");</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>55</v>
+      </c>
+      <c r="B365">
+        <f>ATAN(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C365" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN(0)", "0");</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>55</v>
+      </c>
+      <c r="B366">
+        <f>ATAN(1234)</f>
+        <v>1.5699859542008134</v>
+      </c>
+      <c r="C366" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN(1234)", "1,56998595420081");</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>55</v>
+      </c>
+      <c r="B367">
+        <f>ATAN(PI()/2)</f>
+        <v>1.0038848218538872</v>
+      </c>
+      <c r="C367" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN(PI()/2)", "1,00388482185389");</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>55</v>
+      </c>
+      <c r="B368">
+        <f>ATAN(PI())</f>
+        <v>1.2626272556789118</v>
+      </c>
+      <c r="C368" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN(PI())", "1,26262725567891");</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>55</v>
+      </c>
+      <c r="B369">
+        <f>ATAN(-PI()/3)</f>
+        <v>-0.80844879263002201</v>
+      </c>
+      <c r="C369" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN(-PI()/3)", "-0,808448792630022");</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A370" s="7"/>
+      <c r="B370" s="7"/>
+      <c r="C370" s="8"/>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>56</v>
+      </c>
+      <c r="B371">
+        <f>ATAN2(-2, -2)</f>
+        <v>-2.3561944901923448</v>
+      </c>
+      <c r="C371" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN2(-2, -2)", "-2,35619449019234");</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>56</v>
+      </c>
+      <c r="B372">
+        <f>ATAN2(-1,0)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="C372" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN2(-1,0)", "3,14159265358979");</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>56</v>
+      </c>
+      <c r="B373" t="e">
+        <f>ATAN2(0,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C373" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN2(0,0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>56</v>
+      </c>
+      <c r="B374">
+        <f>ATAN2(0,1)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C374" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN2(0,1)", "1,5707963267949");</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>56</v>
+      </c>
+      <c r="B375">
+        <f>ATAN2(1,2)</f>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="C375" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATAN2(1,2)", "1,10714871779409");</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="7"/>
+      <c r="B376" s="7"/>
+      <c r="C376" s="8"/>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>57</v>
+      </c>
+      <c r="B377">
+        <f>ATANH(-0.99999)</f>
+        <v>-6.1030338227611125</v>
+      </c>
+      <c r="C377" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATANH(-0,99999)", "-6,10303382276111");</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>57</v>
+      </c>
+      <c r="B378" t="e">
+        <f>ATANH(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C378" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATANH(-1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>57</v>
+      </c>
+      <c r="B379">
+        <f>ATANH(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C379" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATANH(0)", "0");</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>57</v>
+      </c>
+      <c r="B380" t="e">
+        <f>ATANH(1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C380" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATANH(1)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>57</v>
+      </c>
+      <c r="B381">
+        <f>ATANH(0.99999)</f>
+        <v>6.1030338227611125</v>
+      </c>
+      <c r="C381" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATANH(0,99999)", "6,10303382276111");</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>57</v>
+      </c>
+      <c r="B382">
+        <f>ATANH(0.233)</f>
+        <v>0.23735935089854404</v>
+      </c>
+      <c r="C382" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=ATANH(0,233)", "0,237359350898544");</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A383" s="7"/>
+      <c r="B383" s="7"/>
+      <c r="C383" s="8"/>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>58</v>
+      </c>
+      <c r="B384">
+        <f>COS(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C384" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(0)", "1");</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>58</v>
+      </c>
+      <c r="B385">
+        <f>COS(1)</f>
+        <v>0.54030230586813977</v>
+      </c>
+      <c r="C385" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(1)", "0,54030230586814");</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>58</v>
+      </c>
+      <c r="B386">
+        <f>COS(2)</f>
+        <v>-0.41614683654714241</v>
+      </c>
+      <c r="C386" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(2)", "-0,416146836547142");</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>58</v>
+      </c>
+      <c r="B387">
+        <f>COS(3)</f>
+        <v>-0.98999249660044542</v>
+      </c>
+      <c r="C387" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(3)", "-0,989992496600445");</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>58</v>
+      </c>
+      <c r="B388">
+        <f>COS(4)</f>
+        <v>-0.65364362086361194</v>
+      </c>
+      <c r="C388" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(4)", "-0,653643620863612");</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>58</v>
+      </c>
+      <c r="B389">
+        <f>COS(-1)</f>
+        <v>0.54030230586813977</v>
+      </c>
+      <c r="C389" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(-1)", "0,54030230586814");</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A390" s="7"/>
+      <c r="B390" s="7"/>
+      <c r="C390" s="8"/>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>59</v>
+      </c>
+      <c r="B391">
+        <f>COSH(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C391" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(0)", "1");</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>59</v>
+      </c>
+      <c r="B392">
+        <f>COSH(1)</f>
+        <v>1.5430806348152437</v>
+      </c>
+      <c r="C392" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(1)", "1,54308063481524");</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>59</v>
+      </c>
+      <c r="B393">
+        <f>COSH(3)</f>
+        <v>10.067661995777765</v>
+      </c>
+      <c r="C393" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(3)", "10,0676619957778");</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>59</v>
+      </c>
+      <c r="B394">
+        <f>COSH(51)</f>
+        <v>7.0467454121346943E+21</v>
+      </c>
+      <c r="C394" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(51)", "7,04674541213469E+21");</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>59</v>
+      </c>
+      <c r="B395">
+        <f>COSH(0.0001)</f>
+        <v>1.000000005</v>
+      </c>
+      <c r="C395" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(0,0001)", "1,000000005");</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>59</v>
+      </c>
+      <c r="B396">
+        <f>COS(-12)</f>
+        <v>0.84385395873249214</v>
+      </c>
+      <c r="C396" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COS(-12)", "0,843853958732492");</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>59</v>
+      </c>
+      <c r="B397" t="e">
+        <f>COSH(-1111111)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C397" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(-1111111)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>59</v>
+      </c>
+      <c r="B398" t="e">
+        <f>COSH(1111111)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C398" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COSH(1111111)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A399" s="7"/>
+      <c r="B399" s="7"/>
+      <c r="C399" s="8"/>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>60</v>
+      </c>
+      <c r="B400" t="e">
+        <f>_xlfn.COT(0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C400" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COT(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>60</v>
+      </c>
+      <c r="B401">
+        <f>_xlfn.COT(-1)</f>
+        <v>-0.64209261593433065</v>
+      </c>
+      <c r="C401" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COT(-1)", "-0,642092615934331");</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>60</v>
+      </c>
+      <c r="B402">
+        <f>_xlfn.COT(1)</f>
+        <v>0.64209261593433065</v>
+      </c>
+      <c r="C402" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COT(1)", "0,642092615934331");</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>60</v>
+      </c>
+      <c r="B403">
+        <f>_xlfn.COT(21)</f>
+        <v>-0.65466511548605755</v>
+      </c>
+      <c r="C403" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COT(21)", "-0,654665115486058");</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>60</v>
+      </c>
+      <c r="B404">
+        <f>_xlfn.COT(0.0001)</f>
+        <v>9999.9999666666663</v>
+      </c>
+      <c r="C404" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COT(0,0001)", "9999,99996666667");</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A405" s="7"/>
+      <c r="B405" s="7"/>
+      <c r="C405" s="8"/>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>61</v>
+      </c>
+      <c r="B406" t="e">
+        <f>_xlfn.COTH(0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C406" s="6" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v>AssertExpression("=COTH(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>61</v>
+      </c>
+      <c r="B407">
+        <f>_xlfn.COTH(1)</f>
+        <v>1.3130352854993315</v>
+      </c>
+      <c r="C407" s="6" t="str">
+        <f t="shared" ref="C407:C434" ca="1" si="25">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B407),"""","\"""),";",","),""", """,IFERROR(B407,IF(ISNA(B407),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=COTH(1)", "1,31303528549933");</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>61</v>
+      </c>
+      <c r="B408">
+        <f>_xlfn.COTH(-10)</f>
+        <v>-1.0000000041223074</v>
+      </c>
+      <c r="C408" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=COTH(-10)", "-1,00000000412231");</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>61</v>
+      </c>
+      <c r="B409">
+        <f>_xlfn.COTH(11)</f>
+        <v>1.0000000005578935</v>
+      </c>
+      <c r="C409" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=COTH(11)", "1,00000000055789");</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>61</v>
+      </c>
+      <c r="B410">
+        <f>_xlfn.COTH(15)</f>
+        <v>1.0000000000001872</v>
+      </c>
+      <c r="C410" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=COTH(15)", "1,00000000000019");</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A411" s="7"/>
+      <c r="B411" s="7"/>
+      <c r="C411" s="8"/>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>62</v>
+      </c>
+      <c r="B412" t="e">
+        <f>_xlfn.CSC(0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C412" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSC(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>62</v>
+      </c>
+      <c r="B413">
+        <f>_xlfn.CSC(1)</f>
+        <v>1.1883951057781212</v>
+      </c>
+      <c r="C413" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSC(1)", "1,18839510577812");</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>62</v>
+      </c>
+      <c r="B414">
+        <f>_xlfn.CSC(-10)</f>
+        <v>1.8381639608896658</v>
+      </c>
+      <c r="C414" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSC(-10)", "1,83816396088967");</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>62</v>
+      </c>
+      <c r="B415">
+        <f>_xlfn.CSC(11)</f>
+        <v>-1.000009793545209</v>
+      </c>
+      <c r="C415" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSC(11)", "-1,00000979354521");</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>62</v>
+      </c>
+      <c r="B416">
+        <f>_xlfn.CSC(15)</f>
+        <v>1.5377805615408537</v>
+      </c>
+      <c r="C416" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSC(15)", "1,53778056154085");</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A417" s="7"/>
+      <c r="B417" s="7"/>
+      <c r="C417" s="8"/>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>63</v>
+      </c>
+      <c r="B418" t="e">
+        <f>_xlfn.CSCH(0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C418" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSCH(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>63</v>
+      </c>
+      <c r="B419">
+        <f>_xlfn.CSCH(1)</f>
+        <v>0.85091812823932156</v>
+      </c>
+      <c r="C419" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSCH(1)", "0,850918128239322");</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>63</v>
+      </c>
+      <c r="B420">
+        <f>_xlfn.CSCH(-10)</f>
+        <v>-9.0799859712122167E-5</v>
+      </c>
+      <c r="C420" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSCH(-10)", "-9,07998597121222E-05");</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>63</v>
+      </c>
+      <c r="B421">
+        <f>_xlfn.CSCH(11)</f>
+        <v>3.3403401589809088E-5</v>
+      </c>
+      <c r="C421" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSCH(11)", "3,34034015898091E-05");</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>63</v>
+      </c>
+      <c r="B422">
+        <f>_xlfn.CSCH(15)</f>
+        <v>6.1180464100370885E-7</v>
+      </c>
+      <c r="C422" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=CSCH(15)", "6,11804641003709E-07");</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A423" s="7"/>
+      <c r="B423" s="7"/>
+      <c r="C423" s="8"/>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>64</v>
+      </c>
+      <c r="B424">
+        <f>_xlfn.SEC(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C424" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SEC(0)", "1");</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>64</v>
+      </c>
+      <c r="B425">
+        <f>_xlfn.SEC(1)</f>
+        <v>1.8508157176809255</v>
+      </c>
+      <c r="C425" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SEC(1)", "1,85081571768093");</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>64</v>
+      </c>
+      <c r="B426">
+        <f>_xlfn.SEC(-10)</f>
+        <v>-1.1917935066878957</v>
+      </c>
+      <c r="C426" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SEC(-10)", "-1,1917935066879");</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>64</v>
+      </c>
+      <c r="B427">
+        <f>_xlfn.SEC(11)</f>
+        <v>225.95305931402496</v>
+      </c>
+      <c r="C427" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SEC(11)", "225,953059314025");</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>64</v>
+      </c>
+      <c r="B428">
+        <f>_xlfn.SEC(15)</f>
+        <v>-1.3163300127243669</v>
+      </c>
+      <c r="C428" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SEC(15)", "-1,31633001272437");</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A429" s="7"/>
+      <c r="B429" s="7"/>
+      <c r="C429" s="8"/>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>65</v>
+      </c>
+      <c r="B430">
+        <f>_xlfn.SECH(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C430" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SECH(0)", "1");</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>65</v>
+      </c>
+      <c r="B431">
+        <f>_xlfn.SECH(1)</f>
+        <v>0.64805427366388546</v>
+      </c>
+      <c r="C431" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SECH(1)", "0,648054273663885");</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>65</v>
+      </c>
+      <c r="B432">
+        <f>_xlfn.SECH(-10)</f>
+        <v>9.0799859337817237E-5</v>
+      </c>
+      <c r="C432" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SECH(-10)", "9,07998593378172E-05");</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>65</v>
+      </c>
+      <c r="B433">
+        <f>_xlfn.SECH(11)</f>
+        <v>3.340340157117355E-5</v>
+      </c>
+      <c r="C433" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SECH(11)", "3,34034015711735E-05");</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>65</v>
+      </c>
+      <c r="B434">
+        <f>_xlfn.SECH(15)</f>
+        <v>6.1180464100359429E-7</v>
+      </c>
+      <c r="C434" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SECH(15)", "6,11804641003594E-07");</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A435" s="7"/>
+      <c r="B435" s="7"/>
+      <c r="C435" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5481,10 +6938,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:H19"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,6 +7131,30 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="e">
+        <f ca="1">SEQUENCE(3.4)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f>{1.2}</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="array" ref="E24">{3;4}</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="array" ref="E25">E23*E24</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added support for ABS, CEILING, CEILING.MATH, CEILING.PRECISE, FLOOR, FLOOR_MATH, FLOOR_PRECISE
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="76">
   <si>
     <t>"A"</t>
   </si>
@@ -224,6 +224,36 @@
   </si>
   <si>
     <t>SECH</t>
+  </si>
+  <si>
+    <t>SIN</t>
+  </si>
+  <si>
+    <t>SINH</t>
+  </si>
+  <si>
+    <t>TAN</t>
+  </si>
+  <si>
+    <t>TANH</t>
+  </si>
+  <si>
+    <t>CEILING</t>
+  </si>
+  <si>
+    <t>CEILING.MATH</t>
+  </si>
+  <si>
+    <t>CEILING.PRECISE</t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>FLOOR.MATH</t>
+  </si>
+  <si>
+    <t>FLOOR.PRECISE</t>
   </si>
 </sst>
 </file>
@@ -1653,15 +1683,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C435"/>
+  <dimension ref="A1:C541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
-      <selection activeCell="C428" sqref="C428"/>
+    <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
+      <selection activeCell="C543" sqref="C543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.5703125" customWidth="1"/>
     <col min="3" max="3" width="72.85546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
@@ -6601,7 +6631,7 @@
         <v>1.3130352854993315</v>
       </c>
       <c r="C407" s="6" t="str">
-        <f t="shared" ref="C407:C434" ca="1" si="25">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B407),"""","\"""),";",","),""", """,IFERROR(B407,IF(ISNA(B407),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C407:C440" ca="1" si="25">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B407),"""","\"""),";",","),""", """,IFERROR(B407,IF(ISNA(B407),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=COTH(1)", "1,31303528549933");</v>
       </c>
     </row>
@@ -6928,6 +6958,1304 @@
       <c r="A435" s="7"/>
       <c r="B435" s="7"/>
       <c r="C435" s="8"/>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>66</v>
+      </c>
+      <c r="B436">
+        <f>SIN(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C436" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SIN(0)", "0");</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>66</v>
+      </c>
+      <c r="B437">
+        <f>SIN(1)</f>
+        <v>0.8414709848078965</v>
+      </c>
+      <c r="C437" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SIN(1)", "0,841470984807897");</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>66</v>
+      </c>
+      <c r="B438">
+        <f>SIN(-10)</f>
+        <v>0.54402111088936977</v>
+      </c>
+      <c r="C438" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SIN(-10)", "0,54402111088937");</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>66</v>
+      </c>
+      <c r="B439">
+        <f>SIN(11)</f>
+        <v>-0.99999020655070348</v>
+      </c>
+      <c r="C439" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SIN(11)", "-0,999990206550703");</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>66</v>
+      </c>
+      <c r="B440">
+        <f>SIN(15)</f>
+        <v>0.65028784015711683</v>
+      </c>
+      <c r="C440" s="6" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v>AssertExpression("=SIN(15)", "0,650287840157117");</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A441" s="7"/>
+      <c r="B441" s="7"/>
+      <c r="C441" s="8"/>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>67</v>
+      </c>
+      <c r="B442">
+        <f>SINH(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C442" s="6" t="str">
+        <f t="shared" ref="C442:C453" ca="1" si="26">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B442),"""","\"""),";",","),""", """,IFERROR(B442,IF(ISNA(B442),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=SINH(0)", "0");</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>67</v>
+      </c>
+      <c r="B443">
+        <f>SINH(1)</f>
+        <v>1.1752011936438014</v>
+      </c>
+      <c r="C443" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=SINH(1)", "1,1752011936438");</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>67</v>
+      </c>
+      <c r="B444">
+        <f>SINH(-10)</f>
+        <v>-11013.232874703393</v>
+      </c>
+      <c r="C444" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=SINH(-10)", "-11013,2328747034");</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>67</v>
+      </c>
+      <c r="B445">
+        <f>SINH(11)</f>
+        <v>29937.070849248059</v>
+      </c>
+      <c r="C445" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=SINH(11)", "29937,0708492481");</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>67</v>
+      </c>
+      <c r="B446">
+        <f>SINH(15)</f>
+        <v>1634508.6862359024</v>
+      </c>
+      <c r="C446" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=SINH(15)", "1634508,6862359");</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A447" s="7"/>
+      <c r="B447" s="7"/>
+      <c r="C447" s="8"/>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>68</v>
+      </c>
+      <c r="B448">
+        <f>TAN(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C448" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=TAN(0)", "0");</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>68</v>
+      </c>
+      <c r="B449">
+        <f>TAN(1)</f>
+        <v>1.5574077246549023</v>
+      </c>
+      <c r="C449" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=TAN(1)", "1,5574077246549");</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>68</v>
+      </c>
+      <c r="B450">
+        <f>TAN(-10)</f>
+        <v>-0.64836082745908663</v>
+      </c>
+      <c r="C450" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=TAN(-10)", "-0,648360827459087");</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>68</v>
+      </c>
+      <c r="B451">
+        <f>TAN(11)</f>
+        <v>-225.95084645419516</v>
+      </c>
+      <c r="C451" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=TAN(11)", "-225,950846454195");</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>68</v>
+      </c>
+      <c r="B452">
+        <f>TAN(PI())</f>
+        <v>-1.22514845490862E-16</v>
+      </c>
+      <c r="C452" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=TAN(PI())", "-1,22514845490862E-16");</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>68</v>
+      </c>
+      <c r="B453">
+        <f>TAN(PI()/2)</f>
+        <v>1.6324552277619072E+16</v>
+      </c>
+      <c r="C453" s="6" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v>AssertExpression("=TAN(PI()/2)", "16324552277619100");</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A454" s="7"/>
+      <c r="B454" s="7"/>
+      <c r="C454" s="8"/>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>69</v>
+      </c>
+      <c r="B455">
+        <f>TANH(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C455" s="6" t="str">
+        <f t="shared" ref="C455:C532" ca="1" si="27">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B455),"""","\"""),";",","),""", """,IFERROR(B455,IF(ISNA(B455),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=TANH(0)", "0");</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>69</v>
+      </c>
+      <c r="B456">
+        <f>TANH(1)</f>
+        <v>0.76159415595576485</v>
+      </c>
+      <c r="C456" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=TANH(1)", "0,761594155955765");</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>69</v>
+      </c>
+      <c r="B457">
+        <f>TANH(-10)</f>
+        <v>-0.99999999587769262</v>
+      </c>
+      <c r="C457" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=TANH(-10)", "-0,999999995877693");</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>69</v>
+      </c>
+      <c r="B458">
+        <f>TANH(11)</f>
+        <v>0.99999999944210649</v>
+      </c>
+      <c r="C458" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=TANH(11)", "0,999999999442106");</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>69</v>
+      </c>
+      <c r="B459">
+        <f>TANH(PI())</f>
+        <v>0.99627207622075009</v>
+      </c>
+      <c r="C459" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=TANH(PI())", "0,99627207622075");</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>69</v>
+      </c>
+      <c r="B460">
+        <f>TANH(PI()/2)</f>
+        <v>0.91715233566727439</v>
+      </c>
+      <c r="C460" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=TANH(PI()/2)", "0,917152335667274");</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A461" s="7"/>
+      <c r="B461" s="7"/>
+      <c r="C461" s="8"/>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>70</v>
+      </c>
+      <c r="B462">
+        <f>CEILING(2.5, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="C462" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING(2,5, 1)", "3");</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>70</v>
+      </c>
+      <c r="B463">
+        <f>CEILING(4, 2)</f>
+        <v>4</v>
+      </c>
+      <c r="C463" s="6" t="str">
+        <f t="shared" ref="C463" ca="1" si="28">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B463),"""","\"""),";",","),""", """,IFERROR(B463,IF(ISNA(B463),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=CEILING(4, 2)", "4");</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>70</v>
+      </c>
+      <c r="B464">
+        <f>CEILING(1234, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C464" s="6" t="str">
+        <f t="shared" ref="C464" ca="1" si="29">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B464),"""","\"""),";",","),""", """,IFERROR(B464,IF(ISNA(B464),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=CEILING(1234, 0)", "0");</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>70</v>
+      </c>
+      <c r="B465">
+        <f>CEILING(-2.5, -2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C465" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING(-2,5, -2)", "-4");</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>70</v>
+      </c>
+      <c r="B466">
+        <f>CEILING(-2.5, 2)</f>
+        <v>-2</v>
+      </c>
+      <c r="C466" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING(-2,5, 2)", "-2");</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>70</v>
+      </c>
+      <c r="B467">
+        <f>CEILING(1.5, 0.1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C467" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING(1,5, 0,1)", "1,5");</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>70</v>
+      </c>
+      <c r="B468">
+        <f>CEILING(-5.5, 2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C468" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING(-5,5, 2)", "-4");</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>70</v>
+      </c>
+      <c r="B469">
+        <f>CEILING(0.234, 0.01)</f>
+        <v>0.24</v>
+      </c>
+      <c r="C469" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING(0,234, 0,01)", "0,24");</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>70</v>
+      </c>
+      <c r="B470">
+        <f>CEILING(1723, 1000)</f>
+        <v>2000</v>
+      </c>
+      <c r="C470" s="6" t="str">
+        <f t="shared" ref="C470" ca="1" si="30">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B470),"""","\"""),";",","),""", """,IFERROR(B470,IF(ISNA(B470),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=CEILING(1723, 1000)", "2000");</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>70</v>
+      </c>
+      <c r="B471">
+        <f>CEILING(12345, 10000)</f>
+        <v>20000</v>
+      </c>
+      <c r="C471" s="6" t="str">
+        <f t="shared" ref="C471" ca="1" si="31">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B471),"""","\"""),";",","),""", """,IFERROR(B471,IF(ISNA(B471),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=CEILING(12345, 10000)", "20000");</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A472" s="7"/>
+      <c r="B472" s="7"/>
+      <c r="C472" s="8"/>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>71</v>
+      </c>
+      <c r="B473">
+        <f>_xlfn.CEILING.MATH(24.3, 5)</f>
+        <v>25</v>
+      </c>
+      <c r="C473" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.MATH(24,3, 5)", "25");</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>71</v>
+      </c>
+      <c r="B474">
+        <f>_xlfn.CEILING.MATH(6.7)</f>
+        <v>7</v>
+      </c>
+      <c r="C474" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.MATH(6,7)", "7");</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>71</v>
+      </c>
+      <c r="B475">
+        <f>_xlfn.CEILING.MATH(-8.1, 2)</f>
+        <v>-8</v>
+      </c>
+      <c r="C475" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.MATH(-8,1, 2)", "-8");</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>71</v>
+      </c>
+      <c r="B476">
+        <f>_xlfn.CEILING.MATH(8.1, 2)</f>
+        <v>10</v>
+      </c>
+      <c r="C476" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.MATH(8,1, 2)", "10");</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>71</v>
+      </c>
+      <c r="B477">
+        <f>_xlfn.CEILING.MATH(-5.5, 2, -1)</f>
+        <v>-6</v>
+      </c>
+      <c r="C477" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.MATH(-5,5, 2, -1)", "-6");</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>71</v>
+      </c>
+      <c r="B478">
+        <f>_xlfn.CEILING.MATH(-5.5, 2, 0)</f>
+        <v>-4</v>
+      </c>
+      <c r="C478" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.MATH(-5,5, 2, 0)", "-4");</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>71</v>
+      </c>
+      <c r="B479">
+        <f>_xlfn.CEILING.MATH(9.99, 10, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="C479" s="6" t="str">
+        <f t="shared" ref="C479:C493" ca="1" si="32">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B479),"""","\"""),";",","),""", """,IFERROR(B479,IF(ISNA(B479),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=CEILING.MATH(9,99, 10, 0)", "10");</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>71</v>
+      </c>
+      <c r="B480">
+        <f>_xlfn.CEILING.MATH(5.2)</f>
+        <v>6</v>
+      </c>
+      <c r="C480" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2)", "6");</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>71</v>
+      </c>
+      <c r="B481">
+        <f>_xlfn.CEILING.MATH(5.2,2)</f>
+        <v>6</v>
+      </c>
+      <c r="C481" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2,2)", "6");</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>71</v>
+      </c>
+      <c r="B482">
+        <f>_xlfn.CEILING.MATH(5.2,-2)</f>
+        <v>6</v>
+      </c>
+      <c r="C482" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2,-2)", "6");</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>71</v>
+      </c>
+      <c r="B483">
+        <f>_xlfn.CEILING.MATH(5.2,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C483" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2,2,0)", "6");</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>71</v>
+      </c>
+      <c r="B484">
+        <f>_xlfn.CEILING.MATH(5.2,2,1)</f>
+        <v>6</v>
+      </c>
+      <c r="C484" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2,2,1)", "6");</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>71</v>
+      </c>
+      <c r="B485">
+        <f>_xlfn.CEILING.MATH(5.2,-2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C485" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2,-2,0)", "6");</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>71</v>
+      </c>
+      <c r="B486">
+        <f>_xlfn.CEILING.MATH(5.2,-2,1)</f>
+        <v>6</v>
+      </c>
+      <c r="C486" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(5,2,-2,1)", "6");</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>71</v>
+      </c>
+      <c r="B487">
+        <f>_xlfn.CEILING.MATH(-5.2)</f>
+        <v>-5</v>
+      </c>
+      <c r="C487" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2)", "-5");</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>71</v>
+      </c>
+      <c r="B488">
+        <f>_xlfn.CEILING.MATH(-5.2,2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C488" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2,2)", "-4");</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>71</v>
+      </c>
+      <c r="B489">
+        <f>_xlfn.CEILING.MATH(-5.2,-2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C489" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2,-2)", "-4");</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>71</v>
+      </c>
+      <c r="B490">
+        <f>_xlfn.CEILING.MATH(-5.2,2,0)</f>
+        <v>-4</v>
+      </c>
+      <c r="C490" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2,2,0)", "-4");</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>71</v>
+      </c>
+      <c r="B491">
+        <f>_xlfn.CEILING.MATH(-5.2,2,1)</f>
+        <v>-6</v>
+      </c>
+      <c r="C491" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2,2,1)", "-6");</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>71</v>
+      </c>
+      <c r="B492">
+        <f>_xlfn.CEILING.MATH(-5.2,-2,0)</f>
+        <v>-4</v>
+      </c>
+      <c r="C492" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2,-2,0)", "-4");</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>71</v>
+      </c>
+      <c r="B493">
+        <f>_xlfn.CEILING.MATH(-5.2,-2,1)</f>
+        <v>-6</v>
+      </c>
+      <c r="C493" s="6" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>AssertExpression("=CEILING.MATH(-5,2,-2,1)", "-6");</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A494" s="7"/>
+      <c r="B494" s="7"/>
+      <c r="C494" s="8"/>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>72</v>
+      </c>
+      <c r="B495">
+        <f>_xlfn.CEILING.PRECISE(4.3)</f>
+        <v>5</v>
+      </c>
+      <c r="C495" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(4,3)", "5");</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>72</v>
+      </c>
+      <c r="B496">
+        <f>_xlfn.CEILING.PRECISE(-4.3)</f>
+        <v>-4</v>
+      </c>
+      <c r="C496" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(-4,3)", "-4");</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>72</v>
+      </c>
+      <c r="B497">
+        <f>_xlfn.CEILING.PRECISE(4.3)</f>
+        <v>5</v>
+      </c>
+      <c r="C497" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(4,3)", "5");</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>72</v>
+      </c>
+      <c r="B498">
+        <f>_xlfn.CEILING.PRECISE(4.3, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="C498" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(4,3, 2)", "6");</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>72</v>
+      </c>
+      <c r="B499">
+        <f>_xlfn.CEILING.PRECISE(4.3, -2)</f>
+        <v>6</v>
+      </c>
+      <c r="C499" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(4,3, -2)", "6");</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>72</v>
+      </c>
+      <c r="B500">
+        <f>_xlfn.CEILING.PRECISE(-4.3, 2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C500" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(-4,3, 2)", "-4");</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>72</v>
+      </c>
+      <c r="B501">
+        <f>_xlfn.CEILING.PRECISE(-4.3, 10)</f>
+        <v>0</v>
+      </c>
+      <c r="C501" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(-4,3, 10)", "0");</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A502" s="7"/>
+      <c r="B502" s="7"/>
+      <c r="C502" s="8"/>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>73</v>
+      </c>
+      <c r="B503">
+        <f>FLOOR(3.7,2)</f>
+        <v>2</v>
+      </c>
+      <c r="C503" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(3,7,2)", "2");</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>73</v>
+      </c>
+      <c r="B504">
+        <f>FLOOR(-2.5,-2)</f>
+        <v>-2</v>
+      </c>
+      <c r="C504" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(-2,5,-2)", "-2");</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>73</v>
+      </c>
+      <c r="B505" t="e">
+        <f>FLOOR(2.5,-2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C505" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(2,5,-2)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>73</v>
+      </c>
+      <c r="B506">
+        <f>FLOOR(-2.5,2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C506" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(-2,5,2)", "-4");</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>73</v>
+      </c>
+      <c r="B507">
+        <f>FLOOR(2.5,2)</f>
+        <v>2</v>
+      </c>
+      <c r="C507" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(2,5,2)", "2");</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>73</v>
+      </c>
+      <c r="B508">
+        <f>FLOOR(1.58,0.1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C508" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(1,58,0,1)", "1,5");</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>73</v>
+      </c>
+      <c r="B509">
+        <f>FLOOR(-1.58,0.1)</f>
+        <v>-1.6</v>
+      </c>
+      <c r="C509" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(-1,58,0,1)", "-1,6");</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>73</v>
+      </c>
+      <c r="B510">
+        <f>FLOOR(0.234,0.01)</f>
+        <v>0.23</v>
+      </c>
+      <c r="C510" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(0,234,0,01)", "0,23");</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>73</v>
+      </c>
+      <c r="B511" t="e">
+        <f>FLOOR(2,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C511" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR(2,0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A512" s="7"/>
+      <c r="B512" s="7"/>
+      <c r="C512" s="8"/>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>74</v>
+      </c>
+      <c r="B513">
+        <f>_xlfn.FLOOR.MATH(24.3,5)</f>
+        <v>20</v>
+      </c>
+      <c r="C513" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(24,3,5)", "20");</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>74</v>
+      </c>
+      <c r="B514">
+        <f>_xlfn.FLOOR.MATH(6.7)</f>
+        <v>6</v>
+      </c>
+      <c r="C514" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(6,7)", "6");</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>74</v>
+      </c>
+      <c r="B515">
+        <f>_xlfn.FLOOR.MATH(-8.1,2)</f>
+        <v>-10</v>
+      </c>
+      <c r="C515" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-8,1,2)", "-10");</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>74</v>
+      </c>
+      <c r="B516">
+        <f>_xlfn.FLOOR.MATH(-5.5,2,-1)</f>
+        <v>-4</v>
+      </c>
+      <c r="C516" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,5,2,-1)", "-4");</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>74</v>
+      </c>
+      <c r="B517">
+        <f>_xlfn.FLOOR.MATH(5.2)</f>
+        <v>5</v>
+      </c>
+      <c r="C517" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2)", "5");</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>74</v>
+      </c>
+      <c r="B518">
+        <f>_xlfn.FLOOR.MATH(5.2,2)</f>
+        <v>4</v>
+      </c>
+      <c r="C518" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2,2)", "4");</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>74</v>
+      </c>
+      <c r="B519">
+        <f>_xlfn.FLOOR.MATH(5.2,-2)</f>
+        <v>4</v>
+      </c>
+      <c r="C519" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2,-2)", "4");</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>74</v>
+      </c>
+      <c r="B520">
+        <f>_xlfn.FLOOR.MATH(5.2,2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C520" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2,2,0)", "4");</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>74</v>
+      </c>
+      <c r="B521">
+        <f>_xlfn.FLOOR.MATH(5.2,2,1)</f>
+        <v>4</v>
+      </c>
+      <c r="C521" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2,2,1)", "4");</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>74</v>
+      </c>
+      <c r="B522">
+        <f>_xlfn.FLOOR.MATH(5.2,-2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C522" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2,-2,0)", "4");</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>74</v>
+      </c>
+      <c r="B523">
+        <f>_xlfn.FLOOR.MATH(5.2,-2,1)</f>
+        <v>4</v>
+      </c>
+      <c r="C523" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(5,2,-2,1)", "4");</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>74</v>
+      </c>
+      <c r="B524">
+        <f>_xlfn.FLOOR.MATH(-5.2)</f>
+        <v>-6</v>
+      </c>
+      <c r="C524" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2)", "-6");</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>74</v>
+      </c>
+      <c r="B525">
+        <f>_xlfn.FLOOR.MATH(-5.2,2)</f>
+        <v>-6</v>
+      </c>
+      <c r="C525" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2,2)", "-6");</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>74</v>
+      </c>
+      <c r="B526">
+        <f>_xlfn.FLOOR.MATH(-5.2,-2)</f>
+        <v>-6</v>
+      </c>
+      <c r="C526" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2,-2)", "-6");</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>74</v>
+      </c>
+      <c r="B527">
+        <f>_xlfn.FLOOR.MATH(-5.2,2,0)</f>
+        <v>-6</v>
+      </c>
+      <c r="C527" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2,2,0)", "-6");</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>74</v>
+      </c>
+      <c r="B528">
+        <f>_xlfn.FLOOR.MATH(-5.2,2,1)</f>
+        <v>-4</v>
+      </c>
+      <c r="C528" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2,2,1)", "-4");</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>74</v>
+      </c>
+      <c r="B529">
+        <f>_xlfn.FLOOR.MATH(-5.2,-2,0)</f>
+        <v>-6</v>
+      </c>
+      <c r="C529" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2,-2,0)", "-6");</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>74</v>
+      </c>
+      <c r="B530">
+        <f>_xlfn.FLOOR.MATH(-5.2,-2,1)</f>
+        <v>-4</v>
+      </c>
+      <c r="C530" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=FLOOR.MATH(-5,2,-2,1)", "-4");</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A531" s="7"/>
+      <c r="B531" s="7"/>
+      <c r="C531" s="8"/>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>75</v>
+      </c>
+      <c r="B532">
+        <f>_xlfn.CEILING.PRECISE(5.2)</f>
+        <v>6</v>
+      </c>
+      <c r="C532" s="6" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>AssertExpression("=CEILING.PRECISE(5,2)", "6");</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>75</v>
+      </c>
+      <c r="B533">
+        <f>_xlfn.CEILING.PRECISE(5.2,2)</f>
+        <v>6</v>
+      </c>
+      <c r="C533" s="6" t="str">
+        <f t="shared" ref="C533:C540" ca="1" si="33">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B533),"""","\"""),";",","),""", """,IFERROR(B533,IF(ISNA(B533),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=CEILING.PRECISE(5,2,2)", "6");</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>75</v>
+      </c>
+      <c r="B534">
+        <f>_xlfn.CEILING.PRECISE(5.2,-2)</f>
+        <v>6</v>
+      </c>
+      <c r="C534" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(5,2,-2)", "6");</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>75</v>
+      </c>
+      <c r="B535">
+        <f>_xlfn.CEILING.PRECISE(-5.2)</f>
+        <v>-5</v>
+      </c>
+      <c r="C535" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(-5,2)", "-5");</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>75</v>
+      </c>
+      <c r="B536">
+        <f>_xlfn.CEILING.PRECISE(-5.2,2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C536" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(-5,2,2)", "-4");</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>75</v>
+      </c>
+      <c r="B537">
+        <f>_xlfn.CEILING.PRECISE(-5.2,-2)</f>
+        <v>-4</v>
+      </c>
+      <c r="C537" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(-5,2,-2)", "-4");</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>75</v>
+      </c>
+      <c r="B538">
+        <f>_xlfn.CEILING.PRECISE(0,-2)</f>
+        <v>0</v>
+      </c>
+      <c r="C538" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(0,-2)", "0");</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>75</v>
+      </c>
+      <c r="B539">
+        <f>_xlfn.CEILING.PRECISE(4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C539" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(4,0)", "0");</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>75</v>
+      </c>
+      <c r="B540">
+        <f>_xlfn.CEILING.PRECISE(0,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C540" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=CEILING.PRECISE(0,0)", "0");</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A541" s="7"/>
+      <c r="B541" s="7"/>
+      <c r="C541" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added support for ROUND, ROUNDUP, ROUNDDOWN, TRUNC, EXP, INT, LN, LOG, LOG10, MOD, POWER, RAND, RANDBETWEEN, SIGN
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="80">
   <si>
     <t>"A"</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>FLOOR.PRECISE</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
+    <t>ROUNDDOWN</t>
+  </si>
+  <si>
+    <t>ROUNDUP</t>
+  </si>
+  <si>
+    <t>TRUNC</t>
   </si>
 </sst>
 </file>
@@ -1683,10 +1695,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C541"/>
+  <dimension ref="A1:C611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
-      <selection activeCell="C543" sqref="C543"/>
+    <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
+      <selection activeCell="B616" sqref="B616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8157,7 +8169,7 @@
         <v>6</v>
       </c>
       <c r="C533" s="6" t="str">
-        <f t="shared" ref="C533:C540" ca="1" si="33">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B533),"""","\"""),";",","),""", """,IFERROR(B533,IF(ISNA(B533),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C533:C596" ca="1" si="33">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B533),"""","\"""),";",","),""", """,IFERROR(B533,IF(ISNA(B533),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=CEILING.PRECISE(5,2,2)", "6");</v>
       </c>
     </row>
@@ -8256,6 +8268,884 @@
       <c r="A541" s="7"/>
       <c r="B541" s="7"/>
       <c r="C541" s="8"/>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>76</v>
+      </c>
+      <c r="B542">
+        <f>ROUND(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C542" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(0, 0)", "0");</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>76</v>
+      </c>
+      <c r="B543">
+        <f>ROUND(10, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="C543" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(10, 0)", "10");</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>76</v>
+      </c>
+      <c r="B544">
+        <f>ROUND(10.001, 2.9)</f>
+        <v>10</v>
+      </c>
+      <c r="C544" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(10,001, 2,9)", "10");</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>76</v>
+      </c>
+      <c r="B545">
+        <f>ROUND(9.99, 2)</f>
+        <v>9.99</v>
+      </c>
+      <c r="C545" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(9,99, 2)", "9,99");</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>76</v>
+      </c>
+      <c r="B546">
+        <f>ROUND(9.999, 2)</f>
+        <v>10</v>
+      </c>
+      <c r="C546" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(9,999, 2)", "10");</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>76</v>
+      </c>
+      <c r="B547">
+        <f>ROUND(-10, 0)</f>
+        <v>-10</v>
+      </c>
+      <c r="C547" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-10, 0)", "-10");</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>76</v>
+      </c>
+      <c r="B548">
+        <f>ROUND(-10, 2)</f>
+        <v>-10</v>
+      </c>
+      <c r="C548" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-10, 2)", "-10");</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>76</v>
+      </c>
+      <c r="B549">
+        <f>ROUND(-9.99, 2)</f>
+        <v>-9.99</v>
+      </c>
+      <c r="C549" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-9,99, 2)", "-9,99");</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>76</v>
+      </c>
+      <c r="B550">
+        <f>ROUND(-9.999, 2)</f>
+        <v>-10</v>
+      </c>
+      <c r="C550" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-9,999, 2)", "-10");</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>76</v>
+      </c>
+      <c r="B551">
+        <f>ROUND(-9.001, 2)</f>
+        <v>-9</v>
+      </c>
+      <c r="C551" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-9,001, 2)", "-9");</v>
+      </c>
+    </row>
+    <row r="552" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>76</v>
+      </c>
+      <c r="B552">
+        <f>ROUND(-9.5, 2)</f>
+        <v>-9.5</v>
+      </c>
+      <c r="C552" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-9,5, 2)", "-9,5");</v>
+      </c>
+    </row>
+    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>76</v>
+      </c>
+      <c r="B553">
+        <f>ROUND(-9.5, 0)</f>
+        <v>-10</v>
+      </c>
+      <c r="C553" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-9,5, 0)", "-10");</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>76</v>
+      </c>
+      <c r="B554">
+        <f>ROUND(9.5, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="C554" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(9,5, 0)", "10");</v>
+      </c>
+    </row>
+    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>76</v>
+      </c>
+      <c r="B555">
+        <f>ROUND(2.15, 1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C555" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(2,15, 1)", "2,2");</v>
+      </c>
+    </row>
+    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>76</v>
+      </c>
+      <c r="B556">
+        <f>ROUND(2.149, 1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="C556" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(2,149, 1)", "2,1");</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>76</v>
+      </c>
+      <c r="B557">
+        <f>ROUND(-1.475, 2)</f>
+        <v>-1.48</v>
+      </c>
+      <c r="C557" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-1,475, 2)", "-1,48");</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>76</v>
+      </c>
+      <c r="B558">
+        <f>ROUND(21.5, -1)</f>
+        <v>20</v>
+      </c>
+      <c r="C558" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(21,5, -1)", "20");</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>76</v>
+      </c>
+      <c r="B559">
+        <f>ROUND(626.3, -3)</f>
+        <v>1000</v>
+      </c>
+      <c r="C559" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(626,3, -3)", "1000");</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>76</v>
+      </c>
+      <c r="B560">
+        <f>ROUND(1.98, -1)</f>
+        <v>0</v>
+      </c>
+      <c r="C560" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(1,98, -1)", "0");</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>76</v>
+      </c>
+      <c r="B561">
+        <f>ROUND(-50.55, -2)</f>
+        <v>-100</v>
+      </c>
+      <c r="C561" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUND(-50,55, -2)", "-100");</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A562" s="7"/>
+      <c r="B562" s="7"/>
+      <c r="C562" s="8"/>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>77</v>
+      </c>
+      <c r="B563">
+        <f>ROUNDDOWN(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C563" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(0, 0)", "0");</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>77</v>
+      </c>
+      <c r="B564">
+        <f>ROUNDDOWN(10, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="C564" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(10, 0)", "10");</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>77</v>
+      </c>
+      <c r="B565">
+        <f>ROUNDDOWN(10.001, 2.9)</f>
+        <v>10</v>
+      </c>
+      <c r="C565" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(10,001, 2,9)", "10");</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>77</v>
+      </c>
+      <c r="B566">
+        <f>ROUNDDOWN(9.99, 2)</f>
+        <v>9.99</v>
+      </c>
+      <c r="C566" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(9,99, 2)", "9,99");</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>77</v>
+      </c>
+      <c r="B567">
+        <f>ROUNDDOWN(9.999, 2)</f>
+        <v>9.99</v>
+      </c>
+      <c r="C567" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(9,999, 2)", "9,99");</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>77</v>
+      </c>
+      <c r="B568">
+        <f>ROUNDDOWN(-10, 0)</f>
+        <v>-10</v>
+      </c>
+      <c r="C568" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-10, 0)", "-10");</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>77</v>
+      </c>
+      <c r="B569">
+        <f>ROUNDDOWN(-10, 2)</f>
+        <v>-10</v>
+      </c>
+      <c r="C569" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-10, 2)", "-10");</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>77</v>
+      </c>
+      <c r="B570">
+        <f>ROUNDDOWN(-9.99, 2)</f>
+        <v>-9.99</v>
+      </c>
+      <c r="C570" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-9,99, 2)", "-9,99");</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>77</v>
+      </c>
+      <c r="B571">
+        <f>ROUNDDOWN(-9.999, 2)</f>
+        <v>-9.99</v>
+      </c>
+      <c r="C571" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-9,999, 2)", "-9,99");</v>
+      </c>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>77</v>
+      </c>
+      <c r="B572">
+        <f>ROUNDDOWN(-9.001, 2)</f>
+        <v>-9</v>
+      </c>
+      <c r="C572" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-9,001, 2)", "-9");</v>
+      </c>
+    </row>
+    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>77</v>
+      </c>
+      <c r="B573">
+        <f>ROUNDDOWN(-9.5, 2)</f>
+        <v>-9.5</v>
+      </c>
+      <c r="C573" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-9,5, 2)", "-9,5");</v>
+      </c>
+    </row>
+    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>77</v>
+      </c>
+      <c r="B574">
+        <f>ROUNDDOWN(-9.5, 0)</f>
+        <v>-9</v>
+      </c>
+      <c r="C574" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-9,5, 0)", "-9");</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>77</v>
+      </c>
+      <c r="B575">
+        <f>ROUNDDOWN(9.5, 0)</f>
+        <v>9</v>
+      </c>
+      <c r="C575" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(9,5, 0)", "9");</v>
+      </c>
+    </row>
+    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>77</v>
+      </c>
+      <c r="B576">
+        <f>ROUNDDOWN(2.15, 1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="C576" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(2,15, 1)", "2,1");</v>
+      </c>
+    </row>
+    <row r="577" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>77</v>
+      </c>
+      <c r="B577">
+        <f>ROUNDDOWN(2.149, 1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="C577" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(2,149, 1)", "2,1");</v>
+      </c>
+    </row>
+    <row r="578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>77</v>
+      </c>
+      <c r="B578">
+        <f>ROUNDDOWN(-1.475, 2)</f>
+        <v>-1.47</v>
+      </c>
+      <c r="C578" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-1,475, 2)", "-1,47");</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>77</v>
+      </c>
+      <c r="B579">
+        <f>ROUNDDOWN(21.5, -1)</f>
+        <v>20</v>
+      </c>
+      <c r="C579" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(21,5, -1)", "20");</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>77</v>
+      </c>
+      <c r="B580">
+        <f>ROUNDDOWN(626.3, -3)</f>
+        <v>0</v>
+      </c>
+      <c r="C580" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(626,3, -3)", "0");</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>77</v>
+      </c>
+      <c r="B581">
+        <f>ROUNDDOWN(1.98, -1)</f>
+        <v>0</v>
+      </c>
+      <c r="C581" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(1,98, -1)", "0");</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>77</v>
+      </c>
+      <c r="B582">
+        <f>ROUNDDOWN(-50.55, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="C582" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDDOWN(-50,55, -2)", "0");</v>
+      </c>
+    </row>
+    <row r="583" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A583" s="7"/>
+      <c r="B583" s="7"/>
+      <c r="C583" s="8"/>
+    </row>
+    <row r="584" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>78</v>
+      </c>
+      <c r="B584">
+        <f>ROUNDUP(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C584" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(0, 0)", "0");</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>78</v>
+      </c>
+      <c r="B585">
+        <f>ROUNDUP(10, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="C585" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(10, 0)", "10");</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>78</v>
+      </c>
+      <c r="B586">
+        <f>ROUNDUP(10.001, 2.9)</f>
+        <v>10.01</v>
+      </c>
+      <c r="C586" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(10,001, 2,9)", "10,01");</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>78</v>
+      </c>
+      <c r="B587">
+        <f>ROUNDUP(9.99, 2)</f>
+        <v>9.99</v>
+      </c>
+      <c r="C587" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(9,99, 2)", "9,99");</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>78</v>
+      </c>
+      <c r="B588">
+        <f>ROUNDUP(9.999, 2)</f>
+        <v>10</v>
+      </c>
+      <c r="C588" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(9,999, 2)", "10");</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>78</v>
+      </c>
+      <c r="B589">
+        <f>ROUNDUP(-10, 0)</f>
+        <v>-10</v>
+      </c>
+      <c r="C589" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-10, 0)", "-10");</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>78</v>
+      </c>
+      <c r="B590">
+        <f>ROUNDUP(-10, 2)</f>
+        <v>-10</v>
+      </c>
+      <c r="C590" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-10, 2)", "-10");</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>78</v>
+      </c>
+      <c r="B591">
+        <f>ROUNDUP(-9.99, 2)</f>
+        <v>-9.99</v>
+      </c>
+      <c r="C591" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-9,99, 2)", "-9,99");</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>78</v>
+      </c>
+      <c r="B592">
+        <f>ROUNDUP(-9.999, 2)</f>
+        <v>-10</v>
+      </c>
+      <c r="C592" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-9,999, 2)", "-10");</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>78</v>
+      </c>
+      <c r="B593">
+        <f>ROUNDUP(-9.001, 2)</f>
+        <v>-9.01</v>
+      </c>
+      <c r="C593" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-9,001, 2)", "-9,01");</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>78</v>
+      </c>
+      <c r="B594">
+        <f>ROUNDUP(-9.5, 2)</f>
+        <v>-9.5</v>
+      </c>
+      <c r="C594" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-9,5, 2)", "-9,5");</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>78</v>
+      </c>
+      <c r="B595">
+        <f>ROUNDUP(-9.5, 0)</f>
+        <v>-10</v>
+      </c>
+      <c r="C595" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(-9,5, 0)", "-10");</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>78</v>
+      </c>
+      <c r="B596">
+        <f>ROUNDUP(9.5, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="C596" s="6" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>AssertExpression("=ROUNDUP(9,5, 0)", "10");</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>78</v>
+      </c>
+      <c r="B597">
+        <f>ROUNDUP(2.15, 1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C597" s="6" t="str">
+        <f t="shared" ref="C597:C610" ca="1" si="34">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B597),"""","\"""),";",","),""", """,IFERROR(B597,IF(ISNA(B597),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=ROUNDUP(2,15, 1)", "2,2");</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>78</v>
+      </c>
+      <c r="B598">
+        <f>ROUNDUP(2.149, 1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C598" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=ROUNDUP(2,149, 1)", "2,2");</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>78</v>
+      </c>
+      <c r="B599">
+        <f>ROUNDUP(-1.475, 2)</f>
+        <v>-1.48</v>
+      </c>
+      <c r="C599" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=ROUNDUP(-1,475, 2)", "-1,48");</v>
+      </c>
+    </row>
+    <row r="600" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>78</v>
+      </c>
+      <c r="B600">
+        <f>ROUNDUP(21.5, -1)</f>
+        <v>30</v>
+      </c>
+      <c r="C600" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=ROUNDUP(21,5, -1)", "30");</v>
+      </c>
+    </row>
+    <row r="601" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>78</v>
+      </c>
+      <c r="B601">
+        <f>ROUNDUP(626.3, -3)</f>
+        <v>1000</v>
+      </c>
+      <c r="C601" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=ROUNDUP(626,3, -3)", "1000");</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>78</v>
+      </c>
+      <c r="B602">
+        <f>ROUNDUP(1.98, -1)</f>
+        <v>10</v>
+      </c>
+      <c r="C602" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=ROUNDUP(1,98, -1)", "10");</v>
+      </c>
+    </row>
+    <row r="603" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>78</v>
+      </c>
+      <c r="B603">
+        <f>ROUNDUP(-50.55, -2)</f>
+        <v>-100</v>
+      </c>
+      <c r="C603" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=ROUNDUP(-50,55, -2)", "-100");</v>
+      </c>
+    </row>
+    <row r="604" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A604" s="7"/>
+      <c r="B604" s="7"/>
+      <c r="C604" s="8"/>
+    </row>
+    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>79</v>
+      </c>
+      <c r="B605">
+        <f>TRUNC(8.9)</f>
+        <v>8</v>
+      </c>
+      <c r="C605" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(8,9)", "8");</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>79</v>
+      </c>
+      <c r="B606">
+        <f>TRUNC(-8.9)</f>
+        <v>-8</v>
+      </c>
+      <c r="C606" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(-8,9)", "-8");</v>
+      </c>
+    </row>
+    <row r="607" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>79</v>
+      </c>
+      <c r="B607">
+        <f>TRUNC(0.45)</f>
+        <v>0</v>
+      </c>
+      <c r="C607" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(0,45)", "0");</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>79</v>
+      </c>
+      <c r="B608">
+        <f>TRUNC(-0.45)</f>
+        <v>0</v>
+      </c>
+      <c r="C608" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(-0,45)", "0");</v>
+      </c>
+    </row>
+    <row r="609" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>79</v>
+      </c>
+      <c r="B609">
+        <f>TRUNC(-0.45, 1)</f>
+        <v>-0.4</v>
+      </c>
+      <c r="C609" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(-0,45, 1)", "-0,4");</v>
+      </c>
+    </row>
+    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>79</v>
+      </c>
+      <c r="B610">
+        <f>TRUNC(0.45, 1)</f>
+        <v>0.4</v>
+      </c>
+      <c r="C610" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(0,45, 1)", "0,4");</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A611" s="7"/>
+      <c r="B611" s="7"/>
+      <c r="C611" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added support for ROWS, COLUMNS, INDEX, LOOKUP
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -15,6 +15,7 @@
     <sheet name="COMPARISON" sheetId="1" r:id="rId1"/>
     <sheet name="TESTS" sheetId="2" r:id="rId2"/>
     <sheet name="DATE" sheetId="3" r:id="rId3"/>
+    <sheet name="JSON" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="168">
   <si>
     <t>"A"</t>
   </si>
@@ -266,6 +267,270 @@
   </si>
   <si>
     <t>TRUNC</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>LOG</t>
+  </si>
+  <si>
+    <t>LOG10</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>RANDBETWEEN</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "expressions": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "name": "F01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "cell": "F3",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "isCollection": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "parent": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "content": ""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "name": "F02",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "cell": "F4",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "content": "_"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "sources": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "name": "N3",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "cell": "N3",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "payload": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "LogHeader": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "Version": "3.10",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "RequestId": "123456",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "Unit": "123"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "RequestData": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "AccountNumber": "923456789012345",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "SEPA": 0.17,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "PS1014": 3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "PS1015": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "PS1016": "MONTH",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "PS1053": "START",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "PS1056": 10000,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "F1041": 5000,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "F1042": 10000,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "InterestTable": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              "Period": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              "Interest": 0.2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              "Points": 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              "Period": 3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              "Interest": 0.25,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              "Points": 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "name": "N4",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "cell": "N4",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "MONTH": "MM",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "YEAR": "YY",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "DAY": "DD"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "name": "N5",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "cell": "N5",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "1": "One",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "2": "Two",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "3": "Three"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "templateName": "T01"</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>expressions</t>
+  </si>
+  <si>
+    <t>isCollection</t>
+  </si>
+  <si>
+    <t>sources</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>templateName</t>
+  </si>
+  <si>
+    <t>T01</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>____</t>
+  </si>
+  <si>
+    <t>[E3:I4]</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -276,7 +541,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +566,16 @@
       <family val="3"/>
       <charset val="161"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +594,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -331,10 +610,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,8 +639,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1695,10 +1977,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C611"/>
+  <dimension ref="A1:C688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
-      <selection activeCell="B616" sqref="B616"/>
+    <sheetView tabSelected="1" topLeftCell="A657" workbookViewId="0">
+      <selection activeCell="B688" sqref="B688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8977,7 +9259,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C597" s="6" t="str">
-        <f t="shared" ref="C597:C610" ca="1" si="34">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B597),"""","\"""),";",","),""", """,IFERROR(B597,IF(ISNA(B597),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C597:C660" ca="1" si="34">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B597),"""","\"""),";",","),""", """,IFERROR(B597,IF(ISNA(B597),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=ROUNDUP(2,15, 1)", "2,2");</v>
       </c>
     </row>
@@ -9095,12 +9377,12 @@
         <v>79</v>
       </c>
       <c r="B607">
-        <f>TRUNC(0.45)</f>
+        <f>TRUNC(0.55)</f>
         <v>0</v>
       </c>
       <c r="C607" s="6" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>AssertExpression("=TRUNC(0,45)", "0");</v>
+        <v>AssertExpression("=TRUNC(0,55)", "0");</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.25">
@@ -9108,12 +9390,12 @@
         <v>79</v>
       </c>
       <c r="B608">
-        <f>TRUNC(-0.45)</f>
+        <f>TRUNC(-0.55)</f>
         <v>0</v>
       </c>
       <c r="C608" s="6" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>AssertExpression("=TRUNC(-0,45)", "0");</v>
+        <v>AssertExpression("=TRUNC(-0,55)", "0");</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
@@ -9121,12 +9403,12 @@
         <v>79</v>
       </c>
       <c r="B609">
-        <f>TRUNC(-0.45, 1)</f>
-        <v>-0.4</v>
+        <f>TRUNC(-0.55, 0)</f>
+        <v>0</v>
       </c>
       <c r="C609" s="6" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>AssertExpression("=TRUNC(-0,45, 1)", "-0,4");</v>
+        <v>AssertExpression("=TRUNC(-0,55, 0)", "0");</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.25">
@@ -9134,18 +9416,935 @@
         <v>79</v>
       </c>
       <c r="B610">
-        <f>TRUNC(0.45, 1)</f>
-        <v>0.4</v>
+        <f>TRUNC(-0.55, -1)</f>
+        <v>0</v>
       </c>
       <c r="C610" s="6" t="str">
+        <f t="shared" ref="C610" ca="1" si="35">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B610),"""","\"""),";",","),""", """,IFERROR(B610,IF(ISNA(B610),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=TRUNC(-0,55, -1)", "0");</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>79</v>
+      </c>
+      <c r="B611">
+        <f>TRUNC(555, -1)</f>
+        <v>550</v>
+      </c>
+      <c r="C611" s="6" t="str">
+        <f t="shared" ref="C611" ca="1" si="36">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B611),"""","\"""),";",","),""", """,IFERROR(B611,IF(ISNA(B611),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=TRUNC(555, -1)", "550");</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>79</v>
+      </c>
+      <c r="B612">
+        <f>TRUNC(555, 1)</f>
+        <v>555</v>
+      </c>
+      <c r="C612" s="6" t="str">
+        <f t="shared" ref="C612" ca="1" si="37">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B612),"""","\"""),";",","),""", """,IFERROR(B612,IF(ISNA(B612),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=TRUNC(555, 1)", "555");</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>79</v>
+      </c>
+      <c r="B613">
+        <f>TRUNC(-0.55, 1)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C613" s="6" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>AssertExpression("=TRUNC(0,45, 1)", "0,4");</v>
-      </c>
-    </row>
-    <row r="611" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A611" s="7"/>
-      <c r="B611" s="7"/>
-      <c r="C611" s="8"/>
+        <v>AssertExpression("=TRUNC(-0,55, 1)", "-0,5");</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>79</v>
+      </c>
+      <c r="B614">
+        <f>TRUNC(0.55, 1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C614" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=TRUNC(0,55, 1)", "0,5");</v>
+      </c>
+    </row>
+    <row r="615" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A615" s="7"/>
+      <c r="B615" s="7"/>
+      <c r="C615" s="8"/>
+    </row>
+    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>80</v>
+      </c>
+      <c r="B616">
+        <f>EXP(0)</f>
+        <v>1</v>
+      </c>
+      <c r="C616" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=EXP(0)", "1");</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>80</v>
+      </c>
+      <c r="B617">
+        <f>EXP(1)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="C617" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=EXP(1)", "2,71828182845905");</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>80</v>
+      </c>
+      <c r="B618">
+        <f>EXP(-1.2)</f>
+        <v>0.30119421191220214</v>
+      </c>
+      <c r="C618" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=EXP(-1,2)", "0,301194211912202");</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>80</v>
+      </c>
+      <c r="B619">
+        <f>EXP(1.234)</f>
+        <v>3.4349418608007598</v>
+      </c>
+      <c r="C619" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=EXP(1,234)", "3,43494186080076");</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A620" s="7"/>
+      <c r="B620" s="7"/>
+      <c r="C620" s="8"/>
+    </row>
+    <row r="621" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>81</v>
+      </c>
+      <c r="B621">
+        <f>INT(0)</f>
+        <v>0</v>
+      </c>
+      <c r="C621" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(0)", "0");</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>81</v>
+      </c>
+      <c r="B622">
+        <f>INT(1.99)</f>
+        <v>1</v>
+      </c>
+      <c r="C622" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(1,99)", "1");</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>81</v>
+      </c>
+      <c r="B623">
+        <f>INT(-1.99)</f>
+        <v>-2</v>
+      </c>
+      <c r="C623" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(-1,99)", "-2");</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>81</v>
+      </c>
+      <c r="B624">
+        <f>INT(-1.5)</f>
+        <v>-2</v>
+      </c>
+      <c r="C624" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(-1,5)", "-2");</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>81</v>
+      </c>
+      <c r="B625">
+        <f>INT(1.5)</f>
+        <v>1</v>
+      </c>
+      <c r="C625" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(1,5)", "1");</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>81</v>
+      </c>
+      <c r="B626">
+        <f>INT(TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="C626" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(TRUE)", "1");</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>81</v>
+      </c>
+      <c r="B627">
+        <f>INT("10,123")</f>
+        <v>10</v>
+      </c>
+      <c r="C627" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=INT(\"10,123\")", "10");</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A628" s="7"/>
+      <c r="B628" s="7"/>
+      <c r="C628" s="8"/>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>82</v>
+      </c>
+      <c r="B629" t="e">
+        <f>LN(0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C629" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LN(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>82</v>
+      </c>
+      <c r="B630">
+        <f>LN(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C630" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LN(1)", "0");</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>82</v>
+      </c>
+      <c r="B631" t="e">
+        <f>LN(-1.2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C631" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LN(-1,2)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>82</v>
+      </c>
+      <c r="B632">
+        <f>LN(1.234)</f>
+        <v>0.21026092548319605</v>
+      </c>
+      <c r="C632" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LN(1,234)", "0,210260925483196");</v>
+      </c>
+    </row>
+    <row r="633" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A633" s="7"/>
+      <c r="B633" s="7"/>
+      <c r="C633" s="8"/>
+    </row>
+    <row r="634" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>83</v>
+      </c>
+      <c r="B634" t="e">
+        <f>LOG(0,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C634" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG(0,2)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>83</v>
+      </c>
+      <c r="B635">
+        <f>LOG(1,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C635" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG(1,2)", "0");</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>83</v>
+      </c>
+      <c r="B636" t="e">
+        <f>LOG(-1.2,2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C636" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG(-1,2,2)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>83</v>
+      </c>
+      <c r="B637">
+        <f>LOG(1.234,2)</f>
+        <v>0.3033423944873308</v>
+      </c>
+      <c r="C637" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG(1,234,2)", "0,303342394487331");</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>83</v>
+      </c>
+      <c r="B638">
+        <f>LOG(5)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="C638" s="6" t="str">
+        <f t="shared" ref="C638:C641" ca="1" si="38">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B638),"""","\"""),";",","),""", """,IFERROR(B638,IF(ISNA(B638),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=LOG(5)", "0,698970004336019");</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>83</v>
+      </c>
+      <c r="B639">
+        <f>LOG(0.599999)</f>
+        <v>-0.2218494734410961</v>
+      </c>
+      <c r="C639" s="6" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>AssertExpression("=LOG(0,599999)", "-0,221849473441096");</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>83</v>
+      </c>
+      <c r="B640">
+        <f>LOG(111111111.9999)</f>
+        <v>8.0457574940346408</v>
+      </c>
+      <c r="C640" s="6" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>AssertExpression("=LOG(111111111,9999)", "8,04575749403464");</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>83</v>
+      </c>
+      <c r="B641">
+        <f>LOG(1.234, 3.2)</f>
+        <v>0.18076841258299328</v>
+      </c>
+      <c r="C641" s="6" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>AssertExpression("=LOG(1,234, 3,2)", "0,180768412582993");</v>
+      </c>
+    </row>
+    <row r="642" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A642" s="7"/>
+      <c r="B642" s="7"/>
+      <c r="C642" s="8"/>
+    </row>
+    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A643" t="s">
+        <v>84</v>
+      </c>
+      <c r="B643" t="e">
+        <f>LOG10(0)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C643" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG10(0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
+        <v>84</v>
+      </c>
+      <c r="B644">
+        <f>LOG10(1)</f>
+        <v>0</v>
+      </c>
+      <c r="C644" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG10(1)", "0");</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
+        <v>84</v>
+      </c>
+      <c r="B645" t="e">
+        <f>LOG10(-1.2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C645" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG10(-1,2)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
+        <v>84</v>
+      </c>
+      <c r="B646">
+        <f>LOG10(1.234)</f>
+        <v>9.131515969722287E-2</v>
+      </c>
+      <c r="C646" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=LOG10(1,234)", "0,0913151596972229");</v>
+      </c>
+    </row>
+    <row r="647" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A647" s="7"/>
+      <c r="B647" s="7"/>
+      <c r="C647" s="8"/>
+    </row>
+    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A648" t="s">
+        <v>85</v>
+      </c>
+      <c r="B648">
+        <f>MOD(0, 5)</f>
+        <v>0</v>
+      </c>
+      <c r="C648" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(0, 5)", "0");</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A649" t="s">
+        <v>85</v>
+      </c>
+      <c r="B649" t="e">
+        <f>MOD(5, 0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C649" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(5, 0)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A650" t="s">
+        <v>85</v>
+      </c>
+      <c r="B650">
+        <f>MOD(5,2)</f>
+        <v>1</v>
+      </c>
+      <c r="C650" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(5,2)", "1");</v>
+      </c>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>85</v>
+      </c>
+      <c r="B651">
+        <f>MOD(10, 1.345)</f>
+        <v>0.58500000000000019</v>
+      </c>
+      <c r="C651" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(10, 1,345)", "0,585");</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A652" t="s">
+        <v>85</v>
+      </c>
+      <c r="B652">
+        <f>MOD(23.456, 2.432)</f>
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="C652" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(23,456, 2,432)", "1,568");</v>
+      </c>
+    </row>
+    <row r="653" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A653" t="s">
+        <v>85</v>
+      </c>
+      <c r="B653">
+        <f>MOD(-23.456, 2.432)</f>
+        <v>0.86399999999999988</v>
+      </c>
+      <c r="C653" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(-23,456, 2,432)", "0,864");</v>
+      </c>
+    </row>
+    <row r="654" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A654" t="s">
+        <v>85</v>
+      </c>
+      <c r="B654">
+        <f>MOD(23.456, -2.432)</f>
+        <v>-0.86399999999999988</v>
+      </c>
+      <c r="C654" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(23,456, -2,432)", "-0,864");</v>
+      </c>
+    </row>
+    <row r="655" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
+        <v>85</v>
+      </c>
+      <c r="B655">
+        <f>MOD(-23.456, -2.432)</f>
+        <v>-1.5680000000000001</v>
+      </c>
+      <c r="C655" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=MOD(-23,456, -2,432)", "-1,568");</v>
+      </c>
+    </row>
+    <row r="656" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A656" s="7"/>
+      <c r="B656" s="7"/>
+      <c r="C656" s="8"/>
+    </row>
+    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
+        <v>86</v>
+      </c>
+      <c r="B657">
+        <f>POWER(0, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="C657" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=POWER(0, 2)", "0");</v>
+      </c>
+    </row>
+    <row r="658" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A658" t="s">
+        <v>86</v>
+      </c>
+      <c r="B658">
+        <f>POWER(1, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="C658" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=POWER(1, 2)", "1");</v>
+      </c>
+    </row>
+    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A659" t="s">
+        <v>86</v>
+      </c>
+      <c r="B659">
+        <f>POWER(-1.2, 2)</f>
+        <v>1.44</v>
+      </c>
+      <c r="C659" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=POWER(-1,2, 2)", "1,44");</v>
+      </c>
+    </row>
+    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A660" t="s">
+        <v>86</v>
+      </c>
+      <c r="B660">
+        <f>POWER(1.234, 2)</f>
+        <v>1.522756</v>
+      </c>
+      <c r="C660" s="6" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>AssertExpression("=POWER(1,234, 2)", "1,522756");</v>
+      </c>
+    </row>
+    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
+        <v>86</v>
+      </c>
+      <c r="B661">
+        <f>POWER(5, -2.34)</f>
+        <v>2.3142495601238641E-2</v>
+      </c>
+      <c r="C661" s="6" t="str">
+        <f t="shared" ref="C661:C673" ca="1" si="39">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B661),"""","\"""),";",","),""", """,IFERROR(B661,IF(ISNA(B661),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=POWER(5, -2,34)", "0,0231424956012386");</v>
+      </c>
+    </row>
+    <row r="662" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
+        <v>86</v>
+      </c>
+      <c r="B662">
+        <f>POWER(0.599999, -1)</f>
+        <v>1.6666694444490742</v>
+      </c>
+      <c r="C662" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=POWER(0,599999, -1)", "1,66666944444907");</v>
+      </c>
+    </row>
+    <row r="663" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A663" t="s">
+        <v>86</v>
+      </c>
+      <c r="B663">
+        <f>POWER(111111111.9999, 1.02)</f>
+        <v>160943204.39223725</v>
+      </c>
+      <c r="C663" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=POWER(111111111,9999, 1,02)", "160943204,392237");</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A664" t="s">
+        <v>86</v>
+      </c>
+      <c r="B664">
+        <f>POWER(1.234, 3.2)</f>
+        <v>1.9597853688279776</v>
+      </c>
+      <c r="C664" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=POWER(1,234, 3,2)", "1,95978536882798");</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A665" s="7"/>
+      <c r="B665" s="7"/>
+      <c r="C665" s="8"/>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A666" t="s">
+        <v>87</v>
+      </c>
+      <c r="B666">
+        <f ca="1">RANDBETWEEN(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C666" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=RANDBETWEEN(0, 0)", "0");</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A667" t="s">
+        <v>87</v>
+      </c>
+      <c r="B667">
+        <f ca="1">RANDBETWEEN(1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="C667" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=RANDBETWEEN(1, 1)", "1");</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
+        <v>87</v>
+      </c>
+      <c r="B668">
+        <f ca="1">RANDBETWEEN(1, 5)</f>
+        <v>4</v>
+      </c>
+      <c r="C668" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=RANDBETWEEN(1, 5)", "4");</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A669" t="s">
+        <v>87</v>
+      </c>
+      <c r="B669" t="e">
+        <f ca="1">RANDBETWEEN(10, 5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C669" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=RANDBETWEEN(10, 5)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
+        <v>87</v>
+      </c>
+      <c r="B670">
+        <f ca="1">RANDBETWEEN(-1.9, 1.9)</f>
+        <v>0</v>
+      </c>
+      <c r="C670" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=RANDBETWEEN(-1,9, 1,9)", "0");</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A671" s="7"/>
+      <c r="B671" s="7">
+        <f t="shared" ref="B671" ca="1" si="40">RANDBETWEEN(-1.9, 1.9)</f>
+        <v>0</v>
+      </c>
+      <c r="C671" s="8"/>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A672" t="s">
+        <v>88</v>
+      </c>
+      <c r="B672">
+        <f>PRODUCT(5,15,30)</f>
+        <v>2250</v>
+      </c>
+      <c r="C672" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=PRODUCT(5,15,30)", "2250");</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A673" t="s">
+        <v>88</v>
+      </c>
+      <c r="B673">
+        <f>PRODUCT({5;15;30}, 2)</f>
+        <v>4500</v>
+      </c>
+      <c r="C673" s="6" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>AssertExpression("=PRODUCT({5,15,30}, 2)", "4500");</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A674" t="s">
+        <v>88</v>
+      </c>
+      <c r="B674">
+        <f>PRODUCT({5;15;30})</f>
+        <v>2250</v>
+      </c>
+      <c r="C674" s="6" t="str">
+        <f t="shared" ref="C674" ca="1" si="41">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B674),"""","\"""),";",","),""", """,IFERROR(B674,IF(ISNA(B674),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=PRODUCT({5,15,30})", "2250");</v>
+      </c>
+    </row>
+    <row r="675" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A675" t="s">
+        <v>88</v>
+      </c>
+      <c r="B675">
+        <f>PRODUCT({5,15,30}, 2)</f>
+        <v>4500</v>
+      </c>
+      <c r="C675" s="6" t="str">
+        <f t="shared" ref="C675" ca="1" si="42">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B675),"""","\"""),";",","),""", """,IFERROR(B675,IF(ISNA(B675),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=PRODUCT({5\15\30}, 2)", "4500");</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A676" t="s">
+        <v>88</v>
+      </c>
+      <c r="B676" t="e">
+        <f>PRODUCT(5,"a",30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C676" s="6" t="str">
+        <f t="shared" ref="C676:C677" ca="1" si="43">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B676),"""","\"""),";",","),""", """,IFERROR(B676,IF(ISNA(B676),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=PRODUCT(5,\"a\",30)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
+        <v>88</v>
+      </c>
+      <c r="B677">
+        <f>PRODUCT({5,"a",30}, 2)</f>
+        <v>300</v>
+      </c>
+      <c r="C677" s="6" t="str">
+        <f t="shared" ca="1" si="43"/>
+        <v>AssertExpression("=PRODUCT({5\\"a\"\30}, 2)", "300");</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A678" t="s">
+        <v>88</v>
+      </c>
+      <c r="B678">
+        <f>PRODUCT({5,15,30}, {5,15,30}, 2)</f>
+        <v>10125000</v>
+      </c>
+      <c r="C678" s="6" t="str">
+        <f t="shared" ref="C678:C686" ca="1" si="44">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B678),"""","\"""),";",","),""", """,IFERROR(B678,IF(ISNA(B678),"#N/A","#VALUE!")),""");")</f>
+        <v>AssertExpression("=PRODUCT({5\15\30}, {5\15\30}, 2)", "10125000");</v>
+      </c>
+    </row>
+    <row r="679" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A679" s="7"/>
+      <c r="B679" s="7"/>
+      <c r="C679" s="8"/>
+    </row>
+    <row r="680" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
+        <v>20</v>
+      </c>
+      <c r="B680">
+        <f>SUM(5,15,30)</f>
+        <v>50</v>
+      </c>
+      <c r="C680" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM(5,15,30)", "50");</v>
+      </c>
+    </row>
+    <row r="681" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A681" t="s">
+        <v>20</v>
+      </c>
+      <c r="B681">
+        <f>SUM({5;15;30}, 2)</f>
+        <v>52</v>
+      </c>
+      <c r="C681" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM({5,15,30}, 2)", "52");</v>
+      </c>
+    </row>
+    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>20</v>
+      </c>
+      <c r="B682">
+        <f>SUM({5;15;30})</f>
+        <v>50</v>
+      </c>
+      <c r="C682" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM({5,15,30})", "50");</v>
+      </c>
+    </row>
+    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
+        <v>20</v>
+      </c>
+      <c r="B683">
+        <f>SUM({5,15,30}, 2)</f>
+        <v>52</v>
+      </c>
+      <c r="C683" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM({5\15\30}, 2)", "52");</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A684" t="s">
+        <v>20</v>
+      </c>
+      <c r="B684" t="e">
+        <f>SUM(5,"a",30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C684" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM(5,\"a\",30)", "#VALUE!");</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A685" t="s">
+        <v>20</v>
+      </c>
+      <c r="B685">
+        <f>SUM({5,"a",30}, 2)</f>
+        <v>37</v>
+      </c>
+      <c r="C685" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM({5\\"a\"\30}, 2)", "37");</v>
+      </c>
+    </row>
+    <row r="686" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
+        <v>20</v>
+      </c>
+      <c r="B686">
+        <f>SUM({5,15,30}, {5,15,30}, 2)</f>
+        <v>102</v>
+      </c>
+      <c r="C686" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=SUM({5\15\30}, {5\15\30}, 2)", "102");</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A687" s="7"/>
+      <c r="B687" s="7"/>
+      <c r="C687" s="8"/>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B688">
+        <f>SUM({5;15;30})</f>
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9376,4 +10575,480 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="77.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="G4" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" t="s">
+        <v>165</v>
+      </c>
+      <c r="L4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" t="s">
+        <v>166</v>
+      </c>
+      <c r="L5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added support for CHOOSE, HLOOKUP, MATCH, VLOOKUP, XLOOKUP
</commit_message>
<xml_diff>
--- a/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
+++ b/DocumentCreator.Tests/Resources/__FunctionTestsHelper.xlsx
@@ -14,9 +14,14 @@
   <sheets>
     <sheet name="COMPARISON" sheetId="1" r:id="rId1"/>
     <sheet name="TESTS" sheetId="2" r:id="rId2"/>
-    <sheet name="DATE" sheetId="3" r:id="rId3"/>
-    <sheet name="JSON" sheetId="4" r:id="rId4"/>
+    <sheet name="CompareTo" sheetId="5" r:id="rId3"/>
+    <sheet name="DATE" sheetId="3" r:id="rId4"/>
+    <sheet name="JSON" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="data1">TESTS!$D$688:$E$689</definedName>
+    <definedName name="data2">TESTS!$D$696:$E$702</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="189">
   <si>
     <t>"A"</t>
   </si>
@@ -531,6 +536,69 @@
   </si>
   <si>
     <t>{}</t>
+  </si>
+  <si>
+    <t>Apples</t>
+  </si>
+  <si>
+    <t>Lemons</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>Pears</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
   </si>
 </sst>
 </file>
@@ -614,7 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -640,6 +708,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -924,7 +993,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1977,10 +2046,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C688"/>
+  <dimension ref="A1:E703"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A657" workbookViewId="0">
-      <selection activeCell="B688" sqref="B688"/>
+    <sheetView tabSelected="1" topLeftCell="A675" workbookViewId="0">
+      <selection activeCell="B696" sqref="B696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10107,11 +10176,11 @@
       </c>
       <c r="B668">
         <f ca="1">RANDBETWEEN(1, 5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C668" s="6" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>AssertExpression("=RANDBETWEEN(1, 5)", "4");</v>
+        <v>AssertExpression("=RANDBETWEEN(1, 5)", "3");</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
@@ -10133,18 +10202,18 @@
       </c>
       <c r="B670">
         <f ca="1">RANDBETWEEN(-1.9, 1.9)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C670" s="6" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>AssertExpression("=RANDBETWEEN(-1,9, 1,9)", "0");</v>
+        <v>AssertExpression("=RANDBETWEEN(-1,9, 1,9)", "-1");</v>
       </c>
     </row>
     <row r="671" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A671" s="7"/>
       <c r="B671" s="7">
         <f t="shared" ref="B671" ca="1" si="40">RANDBETWEEN(-1.9, 1.9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C671" s="8"/>
     </row>
@@ -10161,7 +10230,7 @@
         <v>AssertExpression("=PRODUCT(5,15,30)", "2250");</v>
       </c>
     </row>
-    <row r="673" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
         <v>88</v>
       </c>
@@ -10174,7 +10243,7 @@
         <v>AssertExpression("=PRODUCT({5,15,30}, 2)", "4500");</v>
       </c>
     </row>
-    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
         <v>88</v>
       </c>
@@ -10187,7 +10256,7 @@
         <v>AssertExpression("=PRODUCT({5,15,30})", "2250");</v>
       </c>
     </row>
-    <row r="675" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
         <v>88</v>
       </c>
@@ -10200,7 +10269,7 @@
         <v>AssertExpression("=PRODUCT({5\15\30}, 2)", "4500");</v>
       </c>
     </row>
-    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
         <v>88</v>
       </c>
@@ -10213,7 +10282,7 @@
         <v>AssertExpression("=PRODUCT(5,\"a\",30)", "#VALUE!");</v>
       </c>
     </row>
-    <row r="677" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
         <v>88</v>
       </c>
@@ -10226,7 +10295,7 @@
         <v>AssertExpression("=PRODUCT({5\\"a\"\30}, 2)", "300");</v>
       </c>
     </row>
-    <row r="678" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
         <v>88</v>
       </c>
@@ -10235,16 +10304,16 @@
         <v>10125000</v>
       </c>
       <c r="C678" s="6" t="str">
-        <f t="shared" ref="C678:C686" ca="1" si="44">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B678),"""","\"""),";",","),""", """,IFERROR(B678,IF(ISNA(B678),"#N/A","#VALUE!")),""");")</f>
+        <f t="shared" ref="C678:C702" ca="1" si="44">CONCATENATE("AssertExpression(""",SUBSTITUTE(SUBSTITUTE(_xlfn.FORMULATEXT(B678),"""","\"""),";",","),""", """,IFERROR(B678,IF(ISNA(B678),"#N/A","#VALUE!")),""");")</f>
         <v>AssertExpression("=PRODUCT({5\15\30}, {5\15\30}, 2)", "10125000");</v>
       </c>
     </row>
-    <row r="679" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A679" s="7"/>
       <c r="B679" s="7"/>
       <c r="C679" s="8"/>
     </row>
-    <row r="680" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
         <v>20</v>
       </c>
@@ -10257,7 +10326,7 @@
         <v>AssertExpression("=SUM(5,15,30)", "50");</v>
       </c>
     </row>
-    <row r="681" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
         <v>20</v>
       </c>
@@ -10270,7 +10339,7 @@
         <v>AssertExpression("=SUM({5,15,30}, 2)", "52");</v>
       </c>
     </row>
-    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
         <v>20</v>
       </c>
@@ -10283,7 +10352,7 @@
         <v>AssertExpression("=SUM({5,15,30})", "50");</v>
       </c>
     </row>
-    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
         <v>20</v>
       </c>
@@ -10296,7 +10365,7 @@
         <v>AssertExpression("=SUM({5\15\30}, 2)", "52");</v>
       </c>
     </row>
-    <row r="684" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
         <v>20</v>
       </c>
@@ -10309,7 +10378,7 @@
         <v>AssertExpression("=SUM(5,\"a\",30)", "#VALUE!");</v>
       </c>
     </row>
-    <row r="685" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
         <v>20</v>
       </c>
@@ -10322,7 +10391,7 @@
         <v>AssertExpression("=SUM({5\\"a\"\30}, 2)", "37");</v>
       </c>
     </row>
-    <row r="686" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
         <v>20</v>
       </c>
@@ -10335,16 +10404,256 @@
         <v>AssertExpression("=SUM({5\15\30}, {5\15\30}, 2)", "102");</v>
       </c>
     </row>
-    <row r="687" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A687" s="7"/>
       <c r="B687" s="7"/>
       <c r="C687" s="8"/>
     </row>
-    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B688">
-        <f>SUM({5;15;30})</f>
-        <v>50</v>
-      </c>
+    <row r="688" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A688" t="s">
+        <v>172</v>
+      </c>
+      <c r="B688" t="str">
+        <f t="array" ref="B688">INDEX(data1,0,0)</f>
+        <v>Apples</v>
+      </c>
+      <c r="C688" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("{=INDEX(data1,0,0)}", "Apples");</v>
+      </c>
+      <c r="D688" t="s">
+        <v>168</v>
+      </c>
+      <c r="E688" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="689" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
+        <v>172</v>
+      </c>
+      <c r="B689" t="str">
+        <f t="array" ref="B689">INDEX(data1,1,0)</f>
+        <v>Apples</v>
+      </c>
+      <c r="C689" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("{=INDEX(data1,1,0)}", "Apples");</v>
+      </c>
+      <c r="D689" t="s">
+        <v>170</v>
+      </c>
+      <c r="E689" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="690" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A690" t="s">
+        <v>172</v>
+      </c>
+      <c r="B690" t="str">
+        <f t="array" ref="B690">INDEX(data1,0,1)</f>
+        <v>Apples</v>
+      </c>
+      <c r="C690" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("{=INDEX(data1,0,1)}", "Apples");</v>
+      </c>
+    </row>
+    <row r="691" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
+        <v>172</v>
+      </c>
+      <c r="B691" t="str">
+        <f>INDEX(data1,1,1)</f>
+        <v>Apples</v>
+      </c>
+      <c r="C691" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=INDEX(data1,1,1)", "Apples");</v>
+      </c>
+    </row>
+    <row r="692" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>172</v>
+      </c>
+      <c r="B692" t="str">
+        <f>INDEX(data1,2,2)</f>
+        <v>Pears</v>
+      </c>
+      <c r="C692" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=INDEX(data1,2,2)", "Pears");</v>
+      </c>
+    </row>
+    <row r="693" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>172</v>
+      </c>
+      <c r="B693" t="str">
+        <f t="array" ref="B693">INDEX(data1,2,)</f>
+        <v>Bananas</v>
+      </c>
+      <c r="C693" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("{=INDEX(data1,2,)}", "Bananas");</v>
+      </c>
+    </row>
+    <row r="694" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>172</v>
+      </c>
+      <c r="B694" t="str">
+        <f t="array" ref="B694">INDEX(data1,,2)</f>
+        <v>Lemons</v>
+      </c>
+      <c r="C694" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("{=INDEX(data1,,2)}", "Lemons");</v>
+      </c>
+    </row>
+    <row r="695" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A695" s="7"/>
+      <c r="B695" s="7"/>
+      <c r="C695" s="8"/>
+    </row>
+    <row r="696" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
+        <v>188</v>
+      </c>
+      <c r="B696">
+        <f>VLOOKUP("Brazil", data2, 2, 1)</f>
+        <v>55</v>
+      </c>
+      <c r="C696" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"Brazil\", data2, 2, 1)", "55");</v>
+      </c>
+      <c r="D696" t="s">
+        <v>181</v>
+      </c>
+      <c r="E696">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="697" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>188</v>
+      </c>
+      <c r="B697">
+        <f>VLOOKUP("Brazil", data2, 2, 0)</f>
+        <v>55</v>
+      </c>
+      <c r="C697" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"Brazil\", data2, 2, 0)", "55");</v>
+      </c>
+      <c r="D697" t="s">
+        <v>182</v>
+      </c>
+      <c r="E697">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="698" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A698" t="s">
+        <v>188</v>
+      </c>
+      <c r="B698" t="e">
+        <f>VLOOKUP("Germany", data2, 2, 0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C698" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"Germany\", data2, 2, 0)", "#N/A");</v>
+      </c>
+      <c r="D698" t="s">
+        <v>183</v>
+      </c>
+      <c r="E698">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="699" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A699" t="s">
+        <v>188</v>
+      </c>
+      <c r="B699">
+        <f>VLOOKUP("Malta", data2, 2, 1)</f>
+        <v>62</v>
+      </c>
+      <c r="C699" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"Malta\", data2, 2, 1)", "62");</v>
+      </c>
+      <c r="D699" t="s">
+        <v>184</v>
+      </c>
+      <c r="E699">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="700" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A700" t="s">
+        <v>188</v>
+      </c>
+      <c r="B700">
+        <f>VLOOKUP("*ia", data2, 2, )</f>
+        <v>91</v>
+      </c>
+      <c r="C700" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"*ia\", data2, 2, )", "91");</v>
+      </c>
+      <c r="D700" t="s">
+        <v>185</v>
+      </c>
+      <c r="E700">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="701" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
+        <v>188</v>
+      </c>
+      <c r="B701">
+        <f>VLOOKUP("*?*", data2, 2, )</f>
+        <v>86</v>
+      </c>
+      <c r="C701" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"*?*\", data2, 2, )", "86");</v>
+      </c>
+      <c r="D701" t="s">
+        <v>186</v>
+      </c>
+      <c r="E701">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="702" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A702" t="s">
+        <v>188</v>
+      </c>
+      <c r="B702">
+        <f>VLOOKUP("*e?e", data2, 2, )</f>
+        <v>30</v>
+      </c>
+      <c r="C702" s="6" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>AssertExpression("=VLOOKUP(\"*e?e\", data2, 2, )", "30");</v>
+      </c>
+      <c r="D702" t="s">
+        <v>187</v>
+      </c>
+      <c r="E702">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="703" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A703" s="7"/>
+      <c r="B703" s="7"/>
+      <c r="C703" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10353,6 +10662,139 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>1.0000000000000001E+32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B1:B22">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:H25"/>
@@ -10577,7 +11019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L73"/>
   <sheetViews>

</xml_diff>